<commit_message>
add: more tries to change the result of the clustered topics
</commit_message>
<xml_diff>
--- a/repo/news_data.xlsx
+++ b/repo/news_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1218,25 +1218,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>影／信義區天坑 蔣萬安：將對台北市工地做全面清查</t>
+          <t>工地施作連續壁釀地層下陷  北市信義區驚見15米長天坑</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>社會</t>
+          <t>財經</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。台北市長蔣萬安晚上到場關心並指出，整個狀況控制住以後，會針對台北市的工地，做全面的清查，是不是有這次事件類似的情況，再積極處理。
-蔣萬安表示，工地的部分，市府馬上勒令停工，找出這次地面坍塌的原因，盡快排除，避免坍塌面積持續擴大。這次地層下陷的事件，整起事件會做完整的調查，並且就工地全面檢視，以及營造商的相關紀錄。台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。周邊拉起警戒線提醒民眾注意安全，有民眾在警方協助下，回住處拿東西。記者林伯東／攝影台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。周邊民眾聚集關心。記者林伯東／攝影台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺，晚間坑洞正在持續灌漿，阻止繼續塌陷。記者林伯東／攝影台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。台北市議員許淑華（前右）到場關心民眾。記者林伯東／攝影台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。台北市長蔣萬安（左二）、台北市議員徐巧芯（右二）到場關心。記者林伯東／攝影</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>['地層下陷', '天坑', '蔣萬安']</t>
-        </is>
-      </c>
+          <t>〔記者蔡亞樺／台北報導〕台北市信義區出現天坑！台北市消防局下午3時13分接獲通報，信義區崇德街60巷22號前新建工地旁道路地層下陷（長15公尺、寬3公尺、深度2至3公尺），附近住家門口的2部機車及一部腳踏車瞬間掉進天坑內，幸無人受傷。
+台北市政府表示，目前已疏散鄰近住戶，並劃設警戒線，消防局已先成立現場指揮站，建管處、新工處、道管中心、瓦斯公司、北水處已派員趕赴現場處理。信義區長也已趕抵現場坐鎮指揮，目前評估約有10餘位住戶需要安置。
+台北市建築管理處表示，該案因連續壁施作，已派員至現場了解處理中，目前了解是連續壁滲水，工地正在止水當中，消防局在現場協助鄰房民眾疏散。</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
           <t>2023/05/13</t>
@@ -1244,40 +1241,25 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>udn</t>
+          <t>ltn</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>北市信義區驚現「天坑」 市長蔣萬安作出四點指示</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>社會</t>
-        </is>
-      </c>
+          <t>北市信義區「地層下陷」釀天坑　蔣萬安：全面清查北市工地</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。台北市長蔣萬安（中）到場關心。記者林伯東／攝影台北市信義區崇德街今（13）日下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺，且二度坍塌。台北市長蔣萬安晚上到場關心並作出四點指示。
-蔣萬安表示，市府已在第一時間做出相關的緊急疏散處置，並向同仁作出四點指示。
-第一、安全至上：
-相關緊急應變處置必須儘速地完成，包括疏散、安置等，已媒合旅宿業進行安置，住民入住可依規定申請補助，我們也會盡力將損害降到最低。
-第二、釐清坍塌原因、儘快排除：
-目前了解可能是連續壁滲水的問題，市府會儘速地找出造成地面坍塌的真正原因，並儘快排除，避免坍塌的面積持續擴大。
-第三、事件整體調查：
-就這次地面坍塌的事件，將針對工地的負責營造商，就過去相關建造紀錄整體調查。
-第四、全市工地全面清查：
-崇德街案緊急處置後，將針對台北市興建工程工地作全面清查，避免相關事件重演。
-蔣萬安強調，目前已責成相關局處，務必盡速完成相關緊急應變作為，確保住民、市民的安全，避免讓地面坍塌的損壞再持續擴大，將損害降到最低，全力捍衛市民生命財產安全。
-根據建管處資料顯示，該起工程工地起造人是東禧建設；承造人是華熊營造；監造人是向度聯合建築師事務所，目前則已針對承造人、監造人各開罰新台幣九萬元。</t>
+          <t>台北市信義區崇德街今（13）日下午3點13分，傳出一處新建案工地旁的道路「地層下陷」，馬路上出現一個長15公尺、寬3公尺、深度約4公尺的天坑，摩托車、腳踏車都掉入坑洞，一旁住戶家門口更是危險「懸空」。而台北市長蔣萬安稍早也前往現場勘查，受訪時表示，第一時間就即刻派員前來，相關單位也做了緊急疏散；也強調，當這次事件的緊急處置告一段落之後，會做台北市相關工地的全面清查，了解是否有類似這次地面坍塌的原因，積極做相關處置，目前對廠商及建築師各開罰9萬元，工地勒令停工。蔣萬安表示，初步了解，也聽了相關單位的說明，我們下午3點13分，消防局接收到地方有反應這邊地層下陷，第一時間就即刻派員前來，也趕快連絡了警察局、新工處、建管處、區公所、自來水處、瓦斯公司、台電等相關單位，也做了緊急疏散。蔣萬安指出，也跟指揮官、相關單位來說明，第一、人員安全最重要，所以相關緊急應變的處置必須盡速完成，包括疏散、安置等等，將這次地面坍塌可能造成的損害降到最低；第二、就旁邊的工地，目前了解可能是連續壁滲水問題，已經趕快做了處理，盡速找出坍塌原因，然後盡快排除，避免坍塌面積持續擴大。第三、會就這次地面坍塌事件進行調查，當然也包括工地實施者、營造商過去的相關紀錄；第四、當這次事件的緊急處置告一段落之後，要做台北市相關工地的全面清查，了解是否有類似這次地面坍塌的原因，要積極來做相關處置。蔣萬安表示，「我們現在已經非常努力在做緊急應變、處置，第一時間也盡快的疏散了住戶。我想市民朋友的安全是最重要的，目前還在緊急處置，我想必要的話我們還是希望做預防性疏散」。而台北市土木技師公會理事長莊均緯指出，還要再把崩塌的孔洞填補完成，現在還在灌水當中，水頭差會慢慢達到平衡，而因地質條件屬於沙跟水，因此擔心擋土設施破洞，只要衝破連續壁的洞，勢必擋土牆後面會崩塌，目前要把崩塌的部分用混泥土灌足外，也在開挖面做水平衡，只要水與地下水位一平衡，土沙部分就會靜止，就不會往開挖面流動，防止二次下陷，目前搶救在可控的範圍。莊均緯表示，通常會發生這狀況，是地面本來就有下陷，只是下陷又再造成第二崩塌，灌漿部分還是從最底下往上灌，表層部分基本上還是有些鬆動，需要等水位平衡後，才能達到搶災最終停止的狀態，估計應該都要到凌晨。</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>['北市', '地層下陷', '天坑', '蔣萬安']</t>
+          <t>['蔣萬安', '信義區', '地層下陷']</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1287,31 +1269,25 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>udn</t>
+          <t>ttv</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>北市信義區陷長15公尺深3公尺「天坑」 6單位急赴現場</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>社會</t>
-        </is>
-      </c>
+          <t>最新／疑工程連續壁施工滲水釀天坑 3戶門口地基掏空急灌漿補救</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>台北市信義區崇德街下午出現地層下陷，北市府表示，消防局於15時13分通報，信義區崇德街60巷22號前的新建工地旁道路地層下陷，長15公尺、寬3公尺、深度2至3公尺，無人受傷。
-市府表示，目前處置作為已疏散鄰近住戶，並劃設警戒線，消防局已先成立現場指揮站，建管處、新工處、道管中心、瓦斯公司、北水處已派員趕赴現場處理。信義區區長也已趕抵現場坐鎮指揮。目前評估約有10餘位住戶需要安置。
-北市信義區出現長15公尺、深3公尺「天坑」。圖／北市府提供北市信義區出現長15公尺、深3公尺「天坑」。圖／北市府提供</t>
+          <t>【17：27｜更新天坑初步原因】信義區崇德街今（13）天下午3點13分，傳出一處新建案工地旁的道路「地層下陷」，消防局獲報緊急疏散鄰近住戶、無人受傷。根據消防局獲報消息，信義區崇德街60巷22號前的新建工地旁，出現道路地層下陷，馬路上出現一個長15公尺、寬3公尺、深度約4公尺的天坑，摩托車、腳踏車都掉入坑洞，一旁住戶家門口更是危險「懸空」。警消人員疏散鄰近住戶，所幸無人受傷，目前劃設警戒線，建管處、新工處、道管中心、瓦斯公司、北水處也派員趕赴現場處理，信義區區長已趕抵現場坐鎮指揮，目前評估約有10餘位住戶需要安置。這個天坑幾乎占據整條巷弄，北市建管處初步了解，由於住戶旁就是工地在施工，疑似因為工地連續壁施作，且有出現滲水狀況，才釀成天坑出現，稍早水泥車緊急先進行灌漿作業，主要先基本填補坑洞。受影響住戶也透露，剛剛一度有5名住戶受困在屋子裡，所幸消防員協助救援，而有三戶門口前端地基被掏空，住戶非常擔心房屋可能會倒塌、地基到底穩不穩固、住在裡面到底安不安全、今天晚上到底要住哪裡等問題，不過關於後續賠償等都還要進一步釐清。</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>['北市', '地層下陷', '天坑']</t>
+          <t>['信義區', '地層下陷', '天坑']</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1321,14 +1297,14 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>udn</t>
+          <t>ttv</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>信義區崇德街也出現天坑 消防局布緊戒線疏散鄰近住戶</t>
+          <t>北市信義區疑建案施工釀15公尺坑洞 撤離16戶</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1338,12 +1314,20 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>台北市也出現天坑！今天下午15時許，台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷，坑洞長15公尺、寬3公尺、深度2到3公尺，目視可看到機車、自行車陷落坑中，同時坑洞也波及一旁民宅地基，目前台北市消防局已經疏散鄰近住戶，並劃設緊戒線，並通知府相關單位到場處理。台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷，緊急救援住戶。圖／讀者提供</t>
+          <t>台北市信義區崇德街巷弄內13日下午發生路面塌陷事故，現場緊鄰一旁建案工地。中央社
+台北市信義區一處建案旁的巷弄今天下午出現長15公尺、深3公尺的坑洞，市府表示，正在持續向坑洞灌漿、建案基地灌水，共撤離周遭16戶住戶，其餘住戶判斷沒有危險。
+台北市信義區崇德街巷弄今天下午出現一個長15公尺、寬3公尺、深度3公尺的坑洞，道路緊鄰的建築基地當時正在施作連續壁工程，目前已停工並疏散鄰近住戶，副市長李四川、工務局長黃一平、都發局長王玉芬皆到場了解狀況。
+王玉芬向中央社記者表示，坑洞正在持續灌漿，建築基地則用消防車灌水，讓內外壓力平衡，阻止繼續塌陷，何時才能確認沒有進一步危害則要持續觀察。
+至於住戶部分，王玉芬說，已經撤離16戶，其中有10人需要安置，這些開銷都會由開發單位負責，其餘住戶雖由台北市結構技師公會判斷沒有危險，考量住戶仍會擔心，已請里長逐戶安撫。
+談到事發過程，附近居民仍然餘悸猶存，鄭大哥說，他的姊姊大概下午2時50分的時候聽到「砰」的聲音，並看到門口出現一個小洞，就喊他出去看，洞在這個過程中越來越大，路上的腳踏車、摩托車等就跟著掉下去，「很可怕！」
+鄭大哥表示，他住在這裡3年多了，旁邊的建案大概去年開始施工，剛開挖的時候路面有龜裂，建商就來補好，之後雖然在施工時住家總會感到地震、無法睡午覺，但也沒有什麼異狀。
+黃先生則說，他住這裡20多年了，今天下午在外面散步，走過去時發現有一個小洞，這個洞後來持續陷下去，但他沒有聽到什麼聲音。
+新竹縣竹北莊敬六街一處建案周邊日前才發生路基坍塌，導致一輛停放路邊的特斯拉轎車直接掉落。</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>['北市', '地層下陷', '天坑', '自行車']</t>
+          <t>['北市', '地層下陷', '天坑', '建築', '新竹']</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1360,7 +1344,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>北市信義區工地釀路面現15公尺大天坑 北市府曝原因：連續壁滲水</t>
+          <t>信義區天坑二度坍塌！蔣萬安下令清查北市所有工地 這類遭特別關注</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1369,175 +1353,6 @@
         </is>
       </c>
       <c r="C30" t="inlineStr">
-        <is>
-          <t>台北市信義區一處新建工地旁道路地層下陷，崇德街60巷路面今天下午3點13分出現長15公尺、寬3公尺、約2至3公尺深的大天坑。台北市建管處表示，該案因連續壁施作，已派員至現場了解處理中，目前了解是連續壁滲水，工地正在止水當中，消防局在現場協助鄰房民眾疏散。台北市建管處表示，該案因連續壁施作，已派員至現場了解處理中，工地正在止水當中。圖／讀者提供台北市信義區一處新建工地旁道路地層下陷，崇德街60巷路面出現大天坑。圖／讀者提供</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>['北市', '地層下陷', '天坑']</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>2023/05/13</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>udn</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>北市信義區天坑導致住戶一度受困 現已疏散完畢</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>社會</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>台北市也出現天坑！今天下午15時許，台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷，坑洞長15公尺、寬3公尺、深度2到3公尺，目視可看到機車、自行車陷落坑中，同時坑洞也波及一旁民宅地基，目前台北市消防局已經疏散鄰近住戶10多人，並劃設緊戒線，並通知市府相關單位到場處理。
-天坑位於新建工地及民宅中間巷弄道路，塌陷時發出聲響，驚動住戶，但因為坑洞擋在家門前，第一時間無法脫困，消防局緊急到場，以爬梯方式救援住戶出來。
-消防局救出2名女子，疏散1男1女，人員已全數疏散完畢，另外1名85歲老婦，因長期行動不便，雖無外傷、意識清醒，但家屬要求預防性送醫，由消防局送北醫。由於天坑危及安全，影響周遭至少五戶民宅，部分住戶無法回家，估計有10餘人受影響，將由台北市府處理安置問題。
-台北市信義區出現天坑，目前市府新工處、建管處、勞檢處等相關單位都已派人到場，現場設置指揮所，初步懷疑與民宅對面的新建工地工程有關，現以灌漿方式緊急處置，至於天坑出現原因，將交由市府建管、新工等單位調查。台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>['北市', '地層下陷', '天坑']</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>2023/05/13</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>udn</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>影／信義區工地旁蹋陷緊急灌漿回填 住戶驚慌撤離</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>社會</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>台北市信義區一處新建大樓工地旁巷道，蹋陷，緊急灌漿回填，住戶驚慌撤離 。
-消防局於15時13分獲報，信義區崇德街60巷22號前的新建工地旁道路地層下陷(長15公尺、寬3公尺、深度2~3公尺)，幸無人受傷。
-警消緊急疏散鄰近住戶，並劃設警戒線，消防局已先成立現場指揮站，建管處、新工處、道管中心、瓦斯公司、北水處已派員趕赴現場處理。目前評估約有10餘位住戶需要安置。台北市信義區一處新建大樓工地旁巷道突然塌陷，施工單位緊急灌漿回填，防止塌陷區域擴大 。記者林俊良／攝影警消緊急疏散鄰近住戶，並劃設警戒線，消防局已先成立現場指揮站，目前評估約有10餘位住戶需要安置。記者林俊良／攝影消防局於15時13分獲報，信義區崇德街60巷22號前的新建工地旁道路地層下陷。警消緊急疏散鄰近住戶，並劃設警戒線，消防局已先成立現場指揮站，建管處、新工處、道管中心、瓦斯公司、北水處已派員趕赴現場處理。記者林俊良／攝影今天下午台北市信義區一處新建大樓工地旁巷道，突然塌陷，住戶心有餘悸驚慌撤離，到一旁安全區域。記者林俊良／攝影今天下午台北市信義區一處新建大樓工地旁巷道，突然塌陷，警方疏導住戶驚慌撤離，目前評估約有10餘位住戶需要安置。記者林俊良／攝影台北市信義區一處新建大樓工地旁巷道突然塌陷，施工單位緊急灌漿回填，防止塌陷區域擴大 。記者林俊良／攝影</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>['北市', '地層下陷', '天坑']</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>2023/05/13</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>udn</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>北市信義區民宅前突現天坑 區長：安置補助每人每日1600元</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>社會</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>北市信義區今下午3點多出現大天坑，崇德街60巷民宅前路面坍陷，傍晚5點多坑洞再擴大，消防局已緊急疏散鄰近住戶。信義區公所區長陳冠伶表示，9位有安置需求者，已協助找好旅社並入住，每人每日可申請補助1600元，最多7天。
-區長陳冠伶表示，人數調查一直在變動，目前9位有安置需求，依規定發生緊急災害可申請安置補助，每人一天1600元，最多申請7天，已協助找好旅社，住戶均已入住安置。該坑主要範圍為18號至24號，警戒區12號至24號已拉起封鎖線。台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋／翻攝</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>['北市', '地層下陷', '天坑']</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>2023/05/13</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>udn</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>北市信義區民宅驚見大天坑 市府：撤離16戶、灌漿處理坑洞</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>社會</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>北市信義區崇德街60巷鄰近一處新建工地，今天下午3點多路面突然下陷，出現一個大天坑。台北市副市長李四川、都發局長王玉芬傍晚抵達了解現況，王也說明處理進度，住戶方面已撤離16戶，工程則在坑洞灌漿、建案基地灌水。
-都發局長王玉芬到場表示，馬路上坑洞約10幾公尺長、3公尺寬，深度判斷達到3公尺，以灌漿方式處理。建築基地開挖地下室部分，是用消防水車拉水線灌水，使內外壓力可以平衡，已拉兩條水線，再請消防局再拉一條，加快灌水速度。
-王玉芬說明住戶部分，已經撤離16戶，10人需要安置且安置妥當在某一家旅館，所有住宿、日常開銷都會由營造單位負責；其餘住戶由台北市結構技師公會判斷沒有危險，因居民擔心，也請里長逐戶安撫。現場分為撤離區和監測區，除了天坑之外，轉角一戶有地下室，技師下去看，目前還沒有任何影響，會持續監測。
-黃先生住在當地20多年，他提到走路經過時，有看到裂一個小洞，下午2點多就一直下陷，從22號先坍下去。住戶鄭先生表示，他姊姊騎車來時，突然聽到「砰」一聲被嚇到，那時就有一個小洞，自己也走出去看，前後不到一分鐘出現好大一個洞就停住了，沒多久警察到場就要求不要過去。台北市信義區一處新建大樓工地旁巷道突然塌陷，施工單位緊急灌漿回填，防止塌陷區域擴大 。記者林俊良／攝影</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>['北市', '地層下陷', '天坑']</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>2023/05/13</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>udn</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>信義區天坑二度坍塌！蔣萬安下令清查北市所有工地 這類遭特別關注</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>社會</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
         <is>
           <t>台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。台北市長蔣萬安（中）到場關心。記者林伯東／攝影
 台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。台北市長蔣萬安晚間前往現場，
@@ -1557,169 +1372,354 @@
 台北市信義區崇德街巷弄內道路13日驚傳塌陷，警消獲報到場疏散鄰近住戶，目前無人傷亡。但現場坍塌似有擴大趨勢，傍晚5時許現場再度塌陷，一旁工地藍色帳棚等也遭波及傾倒。中央社台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。圖／消防局提供</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>['地層下陷', '天坑', '蔣萬安']</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>2023/05/13</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>udn</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>北市信義區疑建案施工釀15公尺坑洞 撤離16戶</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>北市信義區民宅驚見大天坑 市府：撤離16戶、灌漿處理坑洞</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>社會</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>台北市信義區崇德街巷弄內13日下午發生路面塌陷事故，現場緊鄰一旁建案工地。中央社
-台北市信義區一處建案旁的巷弄今天下午出現長15公尺、深3公尺的坑洞，市府表示，正在持續向坑洞灌漿、建案基地灌水，共撤離周遭16戶住戶，其餘住戶判斷沒有危險。
-台北市信義區崇德街巷弄今天下午出現一個長15公尺、寬3公尺、深度3公尺的坑洞，道路緊鄰的建築基地當時正在施作連續壁工程，目前已停工並疏散鄰近住戶，副市長李四川、工務局長黃一平、都發局長王玉芬皆到場了解狀況。
-王玉芬向中央社記者表示，坑洞正在持續灌漿，建築基地則用消防車灌水，讓內外壓力平衡，阻止繼續塌陷，何時才能確認沒有進一步危害則要持續觀察。
-至於住戶部分，王玉芬說，已經撤離16戶，其中有10人需要安置，這些開銷都會由開發單位負責，其餘住戶雖由台北市結構技師公會判斷沒有危險，考量住戶仍會擔心，已請里長逐戶安撫。
-談到事發過程，附近居民仍然餘悸猶存，鄭大哥說，他的姊姊大概下午2時50分的時候聽到「砰」的聲音，並看到門口出現一個小洞，就喊他出去看，洞在這個過程中越來越大，路上的腳踏車、摩托車等就跟著掉下去，「很可怕！」
-鄭大哥表示，他住在這裡3年多了，旁邊的建案大概去年開始施工，剛開挖的時候路面有龜裂，建商就來補好，之後雖然在施工時住家總會感到地震、無法睡午覺，但也沒有什麼異狀。
-黃先生則說，他住這裡20多年了，今天下午在外面散步，走過去時發現有一個小洞，這個洞後來持續陷下去，但他沒有聽到什麼聲音。
-新竹縣竹北莊敬六街一處建案周邊日前才發生路基坍塌，導致一輛停放路邊的特斯拉轎車直接掉落。</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>['北市', '地層下陷', '天坑', '建築', '新竹']</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>北市信義區崇德街60巷鄰近一處新建工地，今天下午3點多路面突然下陷，出現一個大天坑。台北市副市長李四川、都發局長王玉芬傍晚抵達了解現況，王也說明處理進度，住戶方面已撤離16戶，工程則在坑洞灌漿、建案基地灌水。
+都發局長王玉芬到場表示，馬路上坑洞約10幾公尺長、3公尺寬，深度判斷達到3公尺，以灌漿方式處理。建築基地開挖地下室部分，是用消防水車拉水線灌水，使內外壓力可以平衡，已拉兩條水線，再請消防局再拉一條，加快灌水速度。
+王玉芬說明住戶部分，已經撤離16戶，10人需要安置且安置妥當在某一家旅館，所有住宿、日常開銷都會由營造單位負責；其餘住戶由台北市結構技師公會判斷沒有危險，因居民擔心，也請里長逐戶安撫。現場分為撤離區和監測區，除了天坑之外，轉角一戶有地下室，技師下去看，目前還沒有任何影響，會持續監測。
+黃先生住在當地20多年，他提到走路經過時，有看到裂一個小洞，下午2點多就一直下陷，從22號先坍下去。住戶鄭先生表示，他姊姊騎車來時，突然聽到「砰」一聲被嚇到，那時就有一個小洞，自己也走出去看，前後不到一分鐘出現好大一個洞就停住了，沒多久警察到場就要求不要過去。台北市信義區一處新建大樓工地旁巷道突然塌陷，施工單位緊急灌漿回填，防止塌陷區域擴大 。記者林俊良／攝影</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>['北市', '地層下陷', '天坑']</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>2023/05/13</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>udn</t>
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>最新／疑工程連續壁施工滲水釀天坑 3戶門口地基掏空急灌漿補救</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>【17：27｜更新天坑初步原因】信義區崇德街今（13）天下午3點13分，傳出一處新建案工地旁的道路「地層下陷」，消防局獲報緊急疏散鄰近住戶、無人受傷。根據消防局獲報消息，信義區崇德街60巷22號前的新建工地旁，出現道路地層下陷，馬路上出現一個長15公尺、寬3公尺、深度約4公尺的天坑，摩托車、腳踏車都掉入坑洞，一旁住戶家門口更是危險「懸空」。警消人員疏散鄰近住戶，所幸無人受傷，目前劃設警戒線，建管處、新工處、道管中心、瓦斯公司、北水處也派員趕赴現場處理，信義區區長已趕抵現場坐鎮指揮，目前評估約有10餘位住戶需要安置。這個天坑幾乎占據整條巷弄，北市建管處初步了解，由於住戶旁就是工地在施工，疑似因為工地連續壁施作，且有出現滲水狀況，才釀成天坑出現，稍早水泥車緊急先進行灌漿作業，主要先基本填補坑洞。受影響住戶也透露，剛剛一度有5名住戶受困在屋子裡，所幸消防員協助救援，而有三戶門口前端地基被掏空，住戶非常擔心房屋可能會倒塌、地基到底穩不穩固、住在裡面到底安不安全、今天晚上到底要住哪裡等問題，不過關於後續賠償等都還要進一步釐清。</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>['信義區', '地層下陷', '天坑']</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>北市信義區民宅前突現天坑 區長：安置補助每人每日1600元</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>社會</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>北市信義區今下午3點多出現大天坑，崇德街60巷民宅前路面坍陷，傍晚5點多坑洞再擴大，消防局已緊急疏散鄰近住戶。信義區公所區長陳冠伶表示，9位有安置需求者，已協助找好旅社並入住，每人每日可申請補助1600元，最多7天。
+區長陳冠伶表示，人數調查一直在變動，目前9位有安置需求，依規定發生緊急災害可申請安置補助，每人一天1600元，最多申請7天，已協助找好旅社，住戶均已入住安置。該坑主要範圍為18號至24號，警戒區12號至24號已拉起封鎖線。台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋／翻攝</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>['北市', '地層下陷', '天坑']</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>2023/05/13</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>ttv</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>北市信義區「地層下陷」釀天坑　蔣萬安：全面清查北市工地</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>台北市信義區崇德街今（13）日下午3點13分，傳出一處新建案工地旁的道路「地層下陷」，馬路上出現一個長15公尺、寬3公尺、深度約4公尺的天坑，摩托車、腳踏車都掉入坑洞，一旁住戶家門口更是危險「懸空」。而台北市長蔣萬安稍早也前往現場勘查，受訪時表示，第一時間就即刻派員前來，相關單位也做了緊急疏散；也強調，當這次事件的緊急處置告一段落之後，會做台北市相關工地的全面清查，了解是否有類似這次地面坍塌的原因，積極做相關處置，目前對廠商及建築師各開罰9萬元，工地勒令停工。蔣萬安表示，初步了解，也聽了相關單位的說明，我們下午3點13分，消防局接收到地方有反應這邊地層下陷，第一時間就即刻派員前來，也趕快連絡了警察局、新工處、建管處、區公所、自來水處、瓦斯公司、台電等相關單位，也做了緊急疏散。蔣萬安指出，也跟指揮官、相關單位來說明，第一、人員安全最重要，所以相關緊急應變的處置必須盡速完成，包括疏散、安置等等，將這次地面坍塌可能造成的損害降到最低；第二、就旁邊的工地，目前了解可能是連續壁滲水問題，已經趕快做了處理，盡速找出坍塌原因，然後盡快排除，避免坍塌面積持續擴大。第三、會就這次地面坍塌事件進行調查，當然也包括工地實施者、營造商過去的相關紀錄；第四、當這次事件的緊急處置告一段落之後，要做台北市相關工地的全面清查，了解是否有類似這次地面坍塌的原因，要積極來做相關處置。蔣萬安表示，「我們現在已經非常努力在做緊急應變、處置，第一時間也盡快的疏散了住戶。我想市民朋友的安全是最重要的，目前還在緊急處置，我想必要的話我們還是希望做預防性疏散」。而台北市土木技師公會理事長莊均緯指出，還要再把崩塌的孔洞填補完成，現在還在灌水當中，水頭差會慢慢達到平衡，而因地質條件屬於沙跟水，因此擔心擋土設施破洞，只要衝破連續壁的洞，勢必擋土牆後面會崩塌，目前要把崩塌的部分用混泥土灌足外，也在開挖面做水平衡，只要水與地下水位一平衡，土沙部分就會靜止，就不會往開挖面流動，防止二次下陷，目前搶救在可控的範圍。莊均緯表示，通常會發生這狀況，是地面本來就有下陷，只是下陷又再造成第二崩塌，灌漿部分還是從最底下往上灌，表層部分基本上還是有些鬆動，需要等水位平衡後，才能達到搶災最終停止的狀態，估計應該都要到凌晨。</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>['蔣萬安', '信義區', '地層下陷']</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>北市信義區天坑導致住戶一度受困 現已疏散完畢</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>社會</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>台北市也出現天坑！今天下午15時許，台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷，坑洞長15公尺、寬3公尺、深度2到3公尺，目視可看到機車、自行車陷落坑中，同時坑洞也波及一旁民宅地基，目前台北市消防局已經疏散鄰近住戶10多人，並劃設緊戒線，並通知市府相關單位到場處理。
+天坑位於新建工地及民宅中間巷弄道路，塌陷時發出聲響，驚動住戶，但因為坑洞擋在家門前，第一時間無法脫困，消防局緊急到場，以爬梯方式救援住戶出來。
+消防局救出2名女子，疏散1男1女，人員已全數疏散完畢，另外1名85歲老婦，因長期行動不便，雖無外傷、意識清醒，但家屬要求預防性送醫，由消防局送北醫。由於天坑危及安全，影響周遭至少五戶民宅，部分住戶無法回家，估計有10餘人受影響，將由台北市府處理安置問題。
+台北市信義區出現天坑，目前市府新工處、建管處、勞檢處等相關單位都已派人到場，現場設置指揮所，初步懷疑與民宅對面的新建工地工程有關，現以灌漿方式緊急處置，至於天坑出現原因，將交由市府建管、新工等單位調查。台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋/翻攝</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>['北市', '地層下陷', '天坑']</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>2023/05/13</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>ttv</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>工地施作連續壁釀地層下陷  北市信義區驚見15米長天坑</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>財經</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>〔記者蔡亞樺／台北報導〕台北市信義區出現天坑！台北市消防局下午3時13分接獲通報，信義區崇德街60巷22號前新建工地旁道路地層下陷（長15公尺、寬3公尺、深度2至3公尺），附近住家門口的2部機車及一部腳踏車瞬間掉進天坑內，幸無人受傷。
-台北市政府表示，目前已疏散鄰近住戶，並劃設警戒線，消防局已先成立現場指揮站，建管處、新工處、道管中心、瓦斯公司、北水處已派員趕赴現場處理。信義區長也已趕抵現場坐鎮指揮，目前評估約有10餘位住戶需要安置。
-台北市建築管理處表示，該案因連續壁施作，已派員至現場了解處理中，目前了解是連續壁滲水，工地正在止水當中，消防局在現場協助鄰房民眾疏散。</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>2023/05/13</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>ltn</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
         <is>
           <t>北市信義區驚見大天坑 市府：勒令停工開罰18萬元</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B34" t="inlineStr">
         <is>
           <t>社會</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>北市信義區崇德街60巷路面今天下午出現大天坑，坑洞長15公尺、寬3公尺、深度2到3公尺，機車、單車陷落坑中，消防局已疏散鄰近住戶10多人。台北市建管處表示，路面坍陷處以混凝土處置，目前已勒令停工，將依建築法開罰營造廠、監造人各9萬元。
 台北市建管處表示，事發地旁為一處新建住宅大樓工地，疑似施作連續壁滲水，導致道路塌陷，目前以混凝土處置，工地現場緊急處理中，將依建築法第89條開罰承造人（營造廠）、監造人（建築師）各9萬元，目前已勒令停工，未來把一切安全問題妥善完成後才會復工。消防局已協助將住戶全部撤離完畢，人員均安全，信義區公所正在處理安置問題。
 北市議員許淑華表示，該處昨晚就在灌水，疑似連續壁施作釀禍，事發地鄰近住戶共30戶，12戶住在坍塌處附近，約10人安置飯店，她也要求市府妥善協助住戶。台北市崇德街出現天坑，警消緊急疏散民眾。記者廖炳棋／翻攝北市信義區出現長15公尺深3公尺「天坑」。圖／北市府提供</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>['北市', '地層下陷', '天坑', '建築', '許淑華']</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2023/05/13</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>北市信義區工地釀路面現15公尺大天坑 北市府曝原因：連續壁滲水</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>社會</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>台北市信義區一處新建工地旁道路地層下陷，崇德街60巷路面今天下午3點13分出現長15公尺、寬3公尺、約2至3公尺深的大天坑。台北市建管處表示，該案因連續壁施作，已派員至現場了解處理中，目前了解是連續壁滲水，工地正在止水當中，消防局在現場協助鄰房民眾疏散。台北市建管處表示，該案因連續壁施作，已派員至現場了解處理中，工地正在止水當中。圖／讀者提供台北市信義區一處新建工地旁道路地層下陷，崇德街60巷路面出現大天坑。圖／讀者提供</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>['北市', '地層下陷', '天坑']</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2023/05/13</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>信義區崇德街也出現天坑 消防局布緊戒線疏散鄰近住戶</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>社會</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>台北市也出現天坑！今天下午15時許，台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷，坑洞長15公尺、寬3公尺、深度2到3公尺，目視可看到機車、自行車陷落坑中，同時坑洞也波及一旁民宅地基，目前台北市消防局已經疏散鄰近住戶，並劃設緊戒線，並通知府相關單位到場處理。台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷。記者廖炳棋/翻攝台北市信義區崇德街60巷22號附近，一處新建工地旁的道路地層下陷，緊急救援住戶。圖／讀者提供</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>['北市', '地層下陷', '天坑', '自行車']</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2023/05/13</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>北市信義區陷長15公尺深3公尺「天坑」 6單位急赴現場</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>社會</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>台北市信義區崇德街下午出現地層下陷，北市府表示，消防局於15時13分通報，信義區崇德街60巷22號前的新建工地旁道路地層下陷，長15公尺、寬3公尺、深度2至3公尺，無人受傷。
+市府表示，目前處置作為已疏散鄰近住戶，並劃設警戒線，消防局已先成立現場指揮站，建管處、新工處、道管中心、瓦斯公司、北水處已派員趕赴現場處理。信義區區長也已趕抵現場坐鎮指揮。目前評估約有10餘位住戶需要安置。
+北市信義區出現長15公尺、深3公尺「天坑」。圖／北市府提供北市信義區出現長15公尺、深3公尺「天坑」。圖／北市府提供</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>['北市', '地層下陷', '天坑']</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2023/05/13</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>北市信義區驚現「天坑」 市長蔣萬安作出四點指示</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>社會</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。台北市長蔣萬安（中）到場關心。記者林伯東／攝影台北市信義區崇德街今（13）日下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺，且二度坍塌。台北市長蔣萬安晚上到場關心並作出四點指示。
+蔣萬安表示，市府已在第一時間做出相關的緊急疏散處置，並向同仁作出四點指示。
+第一、安全至上：
+相關緊急應變處置必須儘速地完成，包括疏散、安置等，已媒合旅宿業進行安置，住民入住可依規定申請補助，我們也會盡力將損害降到最低。
+第二、釐清坍塌原因、儘快排除：
+目前了解可能是連續壁滲水的問題，市府會儘速地找出造成地面坍塌的真正原因，並儘快排除，避免坍塌的面積持續擴大。
+第三、事件整體調查：
+就這次地面坍塌的事件，將針對工地的負責營造商，就過去相關建造紀錄整體調查。
+第四、全市工地全面清查：
+崇德街案緊急處置後，將針對台北市興建工程工地作全面清查，避免相關事件重演。
+蔣萬安強調，目前已責成相關局處，務必盡速完成相關緊急應變作為，確保住民、市民的安全，避免讓地面坍塌的損壞再持續擴大，將損害降到最低，全力捍衛市民生命財產安全。
+根據建管處資料顯示，該起工程工地起造人是東禧建設；承造人是華熊營造；監造人是向度聯合建築師事務所，目前則已針對承造人、監造人各開罰新台幣九萬元。</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>['北市', '地層下陷', '天坑', '蔣萬安']</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2023/05/13</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>影／信義區天坑 蔣萬安：將對台北市工地做全面清查</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>社會</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。台北市長蔣萬安晚上到場關心並指出，整個狀況控制住以後，會針對台北市的工地，做全面的清查，是不是有這次事件類似的情況，再積極處理。
+蔣萬安表示，工地的部分，市府馬上勒令停工，找出這次地面坍塌的原因，盡快排除，避免坍塌面積持續擴大。這次地層下陷的事件，整起事件會做完整的調查，並且就工地全面檢視，以及營造商的相關紀錄。台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。周邊拉起警戒線提醒民眾注意安全，有民眾在警方協助下，回住處拿東西。記者林伯東／攝影台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。周邊民眾聚集關心。記者林伯東／攝影台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺，晚間坑洞正在持續灌漿，阻止繼續塌陷。記者林伯東／攝影台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。台北市議員許淑華（前右）到場關心民眾。記者林伯東／攝影台北市信義區崇德街下午出現地層下陷，天坑長15公尺、寬3公尺、深度2至3公尺。台北市長蔣萬安（左二）、台北市議員徐巧芯（右二）到場關心。記者林伯東／攝影</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>['地層下陷', '天坑', '蔣萬安']</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2023/05/13</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>影／信義區工地旁蹋陷緊急灌漿回填 住戶驚慌撤離</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>社會</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>台北市信義區一處新建大樓工地旁巷道，蹋陷，緊急灌漿回填，住戶驚慌撤離 。
+消防局於15時13分獲報，信義區崇德街60巷22號前的新建工地旁道路地層下陷(長15公尺、寬3公尺、深度2~3公尺)，幸無人受傷。
+警消緊急疏散鄰近住戶，並劃設警戒線，消防局已先成立現場指揮站，建管處、新工處、道管中心、瓦斯公司、北水處已派員趕赴現場處理。目前評估約有10餘位住戶需要安置。台北市信義區一處新建大樓工地旁巷道突然塌陷，施工單位緊急灌漿回填，防止塌陷區域擴大 。記者林俊良／攝影警消緊急疏散鄰近住戶，並劃設警戒線，消防局已先成立現場指揮站，目前評估約有10餘位住戶需要安置。記者林俊良／攝影消防局於15時13分獲報，信義區崇德街60巷22號前的新建工地旁道路地層下陷。警消緊急疏散鄰近住戶，並劃設警戒線，消防局已先成立現場指揮站，建管處、新工處、道管中心、瓦斯公司、北水處已派員趕赴現場處理。記者林俊良／攝影今天下午台北市信義區一處新建大樓工地旁巷道，突然塌陷，住戶心有餘悸驚慌撤離，到一旁安全區域。記者林俊良／攝影今天下午台北市信義區一處新建大樓工地旁巷道，突然塌陷，警方疏導住戶驚慌撤離，目前評估約有10餘位住戶需要安置。記者林俊良／攝影台北市信義區一處新建大樓工地旁巷道突然塌陷，施工單位緊急灌漿回填，防止塌陷區域擴大 。記者林俊良／攝影</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>['北市', '地層下陷', '天坑', '建築', '許淑華']</t>
+          <t>['北市', '地層下陷', '天坑']</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1736,71 +1736,15 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>信義區新建案工地釀路坍 北市將全面會勘地下室開挖工地【更新】</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr"/>
+          <t>台北市信義區「天坑」善後 都發局長王玉芬：住戶回家需符3條件</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>財經</t>
+        </is>
+      </c>
       <c r="C41" t="inlineStr">
-        <is>
-          <t>台北市信義區崇德街一處新建工地旁的道路，13日發生地層下陷，晚間緊急灌漿搶救，晚間11時坑洞初步填平完成，附近住戶一早就跑來關心自己的攤位，擔心會再次坍塌。北市都發局長王玉芬視察表示，初步判斷道路塌陷原因是，因工地地下連續壁約在11至12公尺處有破口，水與砂往地下室流造成坑洞，未來一周將會同三大技師公會全面檢查地下室開挖工地，避免類似意外再度發生。台北市信義區崇德街一處新建工地旁巷道，13日下午突然發生地層下陷，坑洞長約15公尺、寬3公尺、深度3公尺，北市勒令工地停工，附近住戶一早就跑來關心自己的攤位，擔心會再次坍塌。周邊住戶說：「昨晚11、12點還沒睡覺，早上5、6點又趕快跑出來看，也是要關心一下我自己的攤位啊，希望說沒有下一次啦。」信義區區長陳冠伶表示，「安置了5戶，一共是10位，那現在我們把他們都安置在我們信義區的旅館裡。」台北市長蔣萬安上午也前往旅館探視安置戶，致贈慰問金以及康乃馨，報告工程搶修進度。蔣萬安提及，「接下來我們還是要持續監測，第二個我們會請土木技師來做整體評估。」初步了解，因連續壁體滲水造成地下水湧入引發道路坍陷，現場也隨即進行緊急處置，基地外道路下陷處進行灌漿回填，基地內採填砂灌水以平衡水壓。北市府都發局長王玉芬解釋，「初步判斷是工地裡面的地下連續壁，大約在11到12公尺之間有破口，所以它的水跟砂會往地下室裡面流，才造成這個坑洞。」為了避免類似的工地意外再度發生，蔣萬安指出，已責成相關局處針對北市工地全面清查。目前建築工地正在開挖階段有102件，將由三大專業公會逐案現場勘查，於一週內檢查完畢，屆時有安全疑慮者將下令停工、改善。</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>['信義區', '工地', '地下室', '地層下陷', '灌漿', '道路']</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>2023/05/14</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>pts</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>信義區天坑住戶安置「1天補助1600」 建商蓋過101、陶朱隱園</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>北市信義區驚見天坑，市政府表示，坍塌原因指向旁邊的大樓建案，因為地下連續壁有破洞，都發局初步調查後，對承造人和監造人各開出9萬元罰單，等釐清責任歸屬，再進一步開罰。至於附近住戶，目前共10人接受安置，暫住信義區的旅館內，相關費用將由建商來負責。巷弄內路面塌陷好大一塊，深度達到3公尺，一旁民宅門口也遭殃，鐵門幾乎懸空，這樣的情況就發生在台北市信義區，短時間內，房子是不能住了，住戶們該何去何從？台北市信義區長陳冠伶指出，「昨天有做疏散撤離，範圍是從12號到24號，調查結果發現需要安置的住戶一共有5戶」。市府緊急介入安置，一共撤離7戶，需要安置的有5戶，一共10人，暫時住在信義區的旅館內，依照規定，每人每天可以請領的補助金1600元，可以請領7天，但看這情況，住戶們一週內是回不了家了，超出的費用將由建商全額買單。另外，台北市都發局局長王玉芬表示，第一時間已經勒令停工，現在進行的是搶災的部分，同時會對承造人跟監造人，處各9萬元罰鍰。根據初判是建商要負責，因為是一旁的建案施工，地下連續壁破洞釀災，原本要蓋的大樓，地下4層、地上17層，負責營造的華熊營造公司，興建過的包括台北101、世貿中心和陶朱隱園，都是赫赫有名的建築，如今卻發生工安意外，也讓工程暫時喊卡，首要之務得先設法解決安全問題，還給當地居民一個安全的家。</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>['信義區', '天坑', '補助']</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>2023/05/14</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>ttv</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>台北市信義區「天坑」善後 都發局長王玉芬：住戶回家需符3條件</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>財經</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
         <is>
           <t>〔記者楊心慧／台北報導〕台北市信義區崇德街60巷華熊營造建案工地旁的巷道，昨（13）日下午發生地層下陷，出現長15公尺、寬3公尺、深3公尺的巨大坑洞，昨晚灌漿填補坑洞與建案基地，坑洞初步填平完成，但目前為將土水壓平衡，仍在基地內持續灌水；台北市都發局長王玉芬今（14）日上午說明，灌水作業預計今下午完成，至於住戶回家需達3條件，估計作業需1至2週。
 王玉芬今上午抵達現場說明進度，並表示造成道路塌陷初步判斷是工地內的地下連續壁約11、12公尺處有破洞，造成水與砂往工地內流，產生破洞原因，疑似為連續壁施工時有包土狀況，目前已在坑洞進行灌漿回填，基地內則採填砂灌水以平衡水壓。
@@ -1809,30 +1753,30 @@
 台北市信義區長陳冠伶今受訪表示，調查結果撤出的有七戶、需要安置的住戶一共有5戶10人，目前都安置在信義區的旅館內，按照規定發生緊急災害補助可申請安置補助，每人一天1600元，最多可申請七天，超過的部分，廠商承諾超出的部分可負擔。</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr">
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
         <is>
           <t>2023/05/14</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>ltn</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
+    <row r="42">
+      <c r="A42" t="inlineStr">
         <is>
           <t>灌漿8小時填平信義區「天坑」 台北市府預防性疏散安置11人</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>財經</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>首次上稿 00:04更新時間 06:09
 〔記者蔡亞樺／台北報導〕台北市信義區崇德街60巷一處華熊營造建案工地旁的巷道，13日下午3點多發生地層下陷，出現長15公尺、寬3公尺、深3公尺的巨大坑洞，台北市政府與建商展開搶救，灌漿填補坑洞與建案基地，在晚間11點坑洞初步填平完成，北市府啟動預防性疏散，疏散安置11名住戶到旅館住宿。
@@ -1841,7 +1785,63 @@
 虞積學強調，該建案違反「建築法」部分現場已立即勒令停工，並處以18萬元罰鍰，建管處將持續在現場指揮搶救，現場並已要求承商加強設置周遭鄰房安全觀測、提高觀測頻率，直到確認安全無虞。該工地目前已勒令停工，後續須確認週邊地質及鄰房安全無虞，並檢具改善計畫經相關公會審查核可後，始得復工。</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2023/05/14</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>ltn</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>信義區新建案工地釀路坍 北市將全面會勘地下室開挖工地【更新】</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>台北市信義區崇德街一處新建工地旁的道路，13日發生地層下陷，晚間緊急灌漿搶救，晚間11時坑洞初步填平完成，附近住戶一早就跑來關心自己的攤位，擔心會再次坍塌。北市都發局長王玉芬視察表示，初步判斷道路塌陷原因是，因工地地下連續壁約在11至12公尺處有破口，水與砂往地下室流造成坑洞，未來一周將會同三大技師公會全面檢查地下室開挖工地，避免類似意外再度發生。台北市信義區崇德街一處新建工地旁巷道，13日下午突然發生地層下陷，坑洞長約15公尺、寬3公尺、深度3公尺，北市勒令工地停工，附近住戶一早就跑來關心自己的攤位，擔心會再次坍塌。周邊住戶說：「昨晚11、12點還沒睡覺，早上5、6點又趕快跑出來看，也是要關心一下我自己的攤位啊，希望說沒有下一次啦。」信義區區長陳冠伶表示，「安置了5戶，一共是10位，那現在我們把他們都安置在我們信義區的旅館裡。」台北市長蔣萬安上午也前往旅館探視安置戶，致贈慰問金以及康乃馨，報告工程搶修進度。蔣萬安提及，「接下來我們還是要持續監測，第二個我們會請土木技師來做整體評估。」初步了解，因連續壁體滲水造成地下水湧入引發道路坍陷，現場也隨即進行緊急處置，基地外道路下陷處進行灌漿回填，基地內採填砂灌水以平衡水壓。北市府都發局長王玉芬解釋，「初步判斷是工地裡面的地下連續壁，大約在11到12公尺之間有破口，所以它的水跟砂會往地下室裡面流，才造成這個坑洞。」為了避免類似的工地意外再度發生，蔣萬安指出，已責成相關局處針對北市工地全面清查。目前建築工地正在開挖階段有102件，將由三大專業公會逐案現場勘查，於一週內檢查完畢，屆時有安全疑慮者將下令停工、改善。</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>['信義區', '工地', '地下室', '地層下陷', '灌漿', '道路']</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2023/05/14</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>pts</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>信義區天坑住戶安置「1天補助1600」 建商蓋過101、陶朱隱園</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>北市信義區驚見天坑，市政府表示，坍塌原因指向旁邊的大樓建案，因為地下連續壁有破洞，都發局初步調查後，對承造人和監造人各開出9萬元罰單，等釐清責任歸屬，再進一步開罰。至於附近住戶，目前共10人接受安置，暫住信義區的旅館內，相關費用將由建商來負責。巷弄內路面塌陷好大一塊，深度達到3公尺，一旁民宅門口也遭殃，鐵門幾乎懸空，這樣的情況就發生在台北市信義區，短時間內，房子是不能住了，住戶們該何去何從？台北市信義區長陳冠伶指出，「昨天有做疏散撤離，範圍是從12號到24號，調查結果發現需要安置的住戶一共有5戶」。市府緊急介入安置，一共撤離7戶，需要安置的有5戶，一共10人，暫時住在信義區的旅館內，依照規定，每人每天可以請領的補助金1600元，可以請領7天，但看這情況，住戶們一週內是回不了家了，超出的費用將由建商全額買單。另外，台北市都發局局長王玉芬表示，第一時間已經勒令停工，現在進行的是搶災的部分，同時會對承造人跟監造人，處各9萬元罰鍰。根據初判是建商要負責，因為是一旁的建案施工，地下連續壁破洞釀災，原本要蓋的大樓，地下4層、地上17層，負責營造的華熊營造公司，興建過的包括台北101、世貿中心和陶朱隱園，都是赫赫有名的建築，如今卻發生工安意外，也讓工程暫時喊卡，首要之務得先設法解決安全問題，還給當地居民一個安全的家。</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>['信義區', '天坑', '補助']</t>
+        </is>
+      </c>
       <c r="E44" t="inlineStr">
         <is>
           <t>2023/05/14</t>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>ltn</t>
+          <t>ttv</t>
         </is>
       </c>
     </row>
@@ -3295,18 +3295,18 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>【大直民宅坍塌】基泰總經理哭稱委屈　李四川還原現場：有打招呼但沒談任何事</t>
+          <t>【大直民宅坍塌】稱沒收到「超出警戒值」監測資料　北市都發局長公開基泰大直下包商</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr">
         <is>
-          <t>台北市中山區大直民宅塌陷案，基泰建設總經理馮先勉委屈地稱，事發當晚就在現場且站在台北市副市長李四川旁邊。對此，李四川今受訪還原真相，馮當晚的確在現場，但當晚後就沒見到馮到現場關心，還一度失聯找不到人談相關後續事宜。李四川今（11日）接受媒體人王淺秋廣播專訪《千秋萬事》，談及基泰建設董事長陳世銘昨（10日）快閃離開記者會一事，直言碰到問題只能面對、不能逃避。至於基泰總經理馮先勉聲稱一直在現場，李四川則還原，事發當天、7日晚間抵達現場後，一直在處理救災灌水任務，最後因灌水速度不及搶救，他在現場超過約30分鐘後房子才全部沉陷下去。李四川當時就疑惑詢問工地主任「這麼大的事情，你們負責人沒有在現場？只有你一個主任在這？」而工地主任才回應「我們總經理站在旁邊那邊。」李聲稱當下自己不認識馮，且之後也沒見到馮，直至9日救災告一段落、需談安置時，尋找基泰建設的祕書要馮來談一談，結果馮卻沒接電話，連祕書也找不到馮，他才會在媒體前嚴厲譴責基泰。李四川回憶說道，直至10日上午才聯繫到馮先勉，雙方約好9時30分到台北市政府開會，在會同法制局後達成後續的3點承諾。王淺秋詢問，發生事故當晚，工地主任介紹馮先勉後，馮有無過來稍微討論一下發生什麼事？還是馮就在旁邊像個路人一樣圍觀？李四川回應，馮先勉有過來打招呼說自己是總經理，但沒談任何相關事宜。李四川提及當天搶救的緊急過程，當時第一時間緊急疏散住戶且擴大預防性疏散，也聽到消防局回報工地一直傳出有「啪啪啪」聲音，察覺不妥後就要求立即消防局疏散住民，同時也詢問單號住戶對面有無房子間隔，獲得對面還有一排雙號住戶，因此當下就下令對面的也要依法全部撤離，並請區公所找到實踐大學先行安置。李四川當天到現場約22時，當時單號棟已有稍微傾斜、但未沉下去，便立即要求消防局、衛工處、水處全部灌水，看能不能讓基地平衡，不過隨「啪啪啪」間隔時間越來越短，他就要求全部站在旁邊的人全部快疏散。李表示，他在現場約40分鐘後，因灌水無法讓基地平衡，眼睜睜看著房子沉陷，垮掉就等同連續壁全部斷掉，緊急改為灌漿處理。李四川也提及退休後又重新回到北市府工作，很多市政幾乎都不陌生，不過比較麻煩的是極端氣候的影響，市區很多側溝的設計是無法承受近來的豪大雨，若「用工程的技術去追」不斷投入資源改善，怎樣都無法追上老天給的挑戰，舉例豪大雨對一些老舊、低窪的社區，市府要想辦法減災，這也是他回到北市府任職最大的考驗。</t>
+          <t>基泰建設的新建案「基泰大直」因施工不慎釀嚴重公安意外，台北市都發局長王玉芬今日受訪，說明提供3方案供受損嚴峻的25戶長期安置計畫，也公開基泰大直的連續壁廠商為「齊崴營造」。至於本刊揭監測報告早就顯示「已超出警戒值」，王則稱沒看過這份監測報告，後續會要求建商提供。本刊今（11日）獨家揭露，基泰建設委託的儀大工程顧問公司，提供北市都發局7月26日的監測報告顯示，在坍塌前44天的監測報告結論及說明一欄中已明確指出，「部分監測儀器已超出警戒值」，然而基泰建設卻未積極處理，9月照常大規模開挖，最終釀成這起嚴峻公安事故。對此，王玉芬回應，昨（10日）才收到建商提供8、9月的監測報告，7月尚未收到，已要求建商提供完整監測資料，並請專業技師公會判讀，如有發現任何違失，會將技師、建築師等相關人員移送懲戒；媒體追問，判讀需要多少時間？王玉芬回應，由於資料應該很多，但會用最快時間得出結論。除25戶重災戶外，其他居民可返家住，但居民因安全疑慮僅38戶返回。王玉芬稱，近期會召開說明會，由技師公會對所有疑慮的住戶說明檢測結果，以解除住戶疑慮，而這次共撤離236戶民眾，除25戶以外的撤離戶，每戶家中是否有裂縫需要補強，會由技師逐步去勘檢，逐戶記錄去修繕。「我們沒有所謂強迫住戶入住南港社宅，這都是讓住戶可以自己選擇。」王玉芬指出，北市府將於週三（13日）召說明會，說明長期安置的3個方案，包含南港國宅備妥25戶，內有家具、冷氣、冰箱等；若想住在附近，會持續提供安置的旅館；最後民眾可自由選擇居住地，1坪補貼1,600元租金。此外，王玉芬指出，今日已啟動4大技師公會對184處開挖工地進行嚴格檢查，第二波是針對地下室有開挖導溝、連續壁工程檢查，另對所有工地加強加強頻率檢查，預計每月1次，有地下室開挖的會增加檢查頻率，而鄰損規則、SOP結構外審的規定會做一個整體的檢視，即刻啟動修法。王玉芬強調，未來只要建設公司、營造廠或分包廠商、相關技師，有工地涉及公安跟鄰損的，嚴重時就會全部公開資訊，包括下包廠商。而她今日也公布「基泰大直」的下包連續壁廠商為「齊崴營造」，「一個都不要跑掉，也讓大家可以避開雷區。」</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>['台北', '地層下陷', '馮先勉', '基泰建設', '李四川', '大直']</t>
+          <t>['都發局', '租金補貼', '台北', '基泰建設', '大直', '地層下陷', '受災戶', '國宅', '北市府', '建商']</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -3323,18 +3323,18 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>【大直民宅坍塌】稱沒收到「超出警戒值」監測資料　北市都發局長公開基泰大直下包商</t>
+          <t>【監測報告曝人禍2】基泰老董請辭　王世堅：今加告殺人未遂</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr">
         <is>
-          <t>基泰建設的新建案「基泰大直」因施工不慎釀嚴重公安意外，台北市都發局長王玉芬今日受訪，說明提供3方案供受損嚴峻的25戶長期安置計畫，也公開基泰大直的連續壁廠商為「齊崴營造」。至於本刊揭監測報告早就顯示「已超出警戒值」，王則稱沒看過這份監測報告，後續會要求建商提供。本刊今（11日）獨家揭露，基泰建設委託的儀大工程顧問公司，提供北市都發局7月26日的監測報告顯示，在坍塌前44天的監測報告結論及說明一欄中已明確指出，「部分監測儀器已超出警戒值」，然而基泰建設卻未積極處理，9月照常大規模開挖，最終釀成這起嚴峻公安事故。對此，王玉芬回應，昨（10日）才收到建商提供8、9月的監測報告，7月尚未收到，已要求建商提供完整監測資料，並請專業技師公會判讀，如有發現任何違失，會將技師、建築師等相關人員移送懲戒；媒體追問，判讀需要多少時間？王玉芬回應，由於資料應該很多，但會用最快時間得出結論。除25戶重災戶外，其他居民可返家住，但居民因安全疑慮僅38戶返回。王玉芬稱，近期會召開說明會，由技師公會對所有疑慮的住戶說明檢測結果，以解除住戶疑慮，而這次共撤離236戶民眾，除25戶以外的撤離戶，每戶家中是否有裂縫需要補強，會由技師逐步去勘檢，逐戶記錄去修繕。「我們沒有所謂強迫住戶入住南港社宅，這都是讓住戶可以自己選擇。」王玉芬指出，北市府將於週三（13日）召說明會，說明長期安置的3個方案，包含南港國宅備妥25戶，內有家具、冷氣、冰箱等；若想住在附近，會持續提供安置的旅館；最後民眾可自由選擇居住地，1坪補貼1,600元租金。此外，王玉芬指出，今日已啟動4大技師公會對184處開挖工地進行嚴格檢查，第二波是針對地下室有開挖導溝、連續壁工程檢查，另對所有工地加強加強頻率檢查，預計每月1次，有地下室開挖的會增加檢查頻率，而鄰損規則、SOP結構外審的規定會做一個整體的檢視，即刻啟動修法。王玉芬強調，未來只要建設公司、營造廠或分包廠商、相關技師，有工地涉及公安跟鄰損的，嚴重時就會全部公開資訊，包括下包廠商。而她今日也公布「基泰大直」的下包連續壁廠商為「齊崴營造」，「一個都不要跑掉，也讓大家可以避開雷區。」</t>
+          <t>北市基泰大直建案釀成民宅傾斜下陷案，基泰建設昨（10日）在證交所召開重訊記者會，董事長陳世銘在道歉後宣布請辭負責便離去，北市議員王世堅指出，從監測資料判斷，基泰大直在連續壁施作後保養期間，就已出現監測數據異常，基泰仍選擇繼續開挖，業者的「不確定故意」釀成大禍，今（11日）上午11點他將與議員陳怡君共赴北檢加告基泰負責人殺人未遂。王世堅說，基泰大直這類建案，依規定進行深開挖工程前，建商必須安裝監測系統，並記錄每日施工導致各種建物、馬路位移等情況，依照議員陳怡君的會勘紀錄，附近居民檢舉已8個月，市府卻一再回應安全無虞，從監測資料，就可推斷市府的回報是否有行政怠惰、瀆職或疏於監督。「建商老闆是起造人，出了事怎麼可能讓他拍拍屁股就走人！」王世堅說，基泰董事長陳世銘昨天請辭，擺明就是只想用民事賠償解決，不想負刑事責任，他今天將赴北檢加告殺人未遂，就是希望檢方要儘快蒐證，確保事件發生時的起造人應負起完全責任，不能出了事就落跑。</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>['都發局', '租金補貼', '台北', '基泰建設', '大直', '地層下陷', '受災戶', '國宅', '北市府', '建商']</t>
+          <t>['陳世銘', '建商', '陳怡君', '檢察官', '台北', '基泰建設', '大直', '王世堅', '地層下陷', '殺人未遂']</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3351,18 +3351,18 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>【監測報告曝人禍2】基泰老董請辭　王世堅：今加告殺人未遂</t>
+          <t>【大直民宅坍塌】基泰總經理哭稱委屈　李四川還原現場：有打招呼但沒談任何事</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr">
         <is>
-          <t>北市基泰大直建案釀成民宅傾斜下陷案，基泰建設昨（10日）在證交所召開重訊記者會，董事長陳世銘在道歉後宣布請辭負責便離去，北市議員王世堅指出，從監測資料判斷，基泰大直在連續壁施作後保養期間，就已出現監測數據異常，基泰仍選擇繼續開挖，業者的「不確定故意」釀成大禍，今（11日）上午11點他將與議員陳怡君共赴北檢加告基泰負責人殺人未遂。王世堅說，基泰大直這類建案，依規定進行深開挖工程前，建商必須安裝監測系統，並記錄每日施工導致各種建物、馬路位移等情況，依照議員陳怡君的會勘紀錄，附近居民檢舉已8個月，市府卻一再回應安全無虞，從監測資料，就可推斷市府的回報是否有行政怠惰、瀆職或疏於監督。「建商老闆是起造人，出了事怎麼可能讓他拍拍屁股就走人！」王世堅說，基泰董事長陳世銘昨天請辭，擺明就是只想用民事賠償解決，不想負刑事責任，他今天將赴北檢加告殺人未遂，就是希望檢方要儘快蒐證，確保事件發生時的起造人應負起完全責任，不能出了事就落跑。</t>
+          <t>台北市中山區大直民宅塌陷案，基泰建設總經理馮先勉委屈地稱，事發當晚就在現場且站在台北市副市長李四川旁邊。對此，李四川今受訪還原真相，馮當晚的確在現場，但當晚後就沒見到馮到現場關心，還一度失聯找不到人談相關後續事宜。李四川今（11日）接受媒體人王淺秋廣播專訪《千秋萬事》，談及基泰建設董事長陳世銘昨（10日）快閃離開記者會一事，直言碰到問題只能面對、不能逃避。至於基泰總經理馮先勉聲稱一直在現場，李四川則還原，事發當天、7日晚間抵達現場後，一直在處理救災灌水任務，最後因灌水速度不及搶救，他在現場超過約30分鐘後房子才全部沉陷下去。李四川當時就疑惑詢問工地主任「這麼大的事情，你們負責人沒有在現場？只有你一個主任在這？」而工地主任才回應「我們總經理站在旁邊那邊。」李聲稱當下自己不認識馮，且之後也沒見到馮，直至9日救災告一段落、需談安置時，尋找基泰建設的祕書要馮來談一談，結果馮卻沒接電話，連祕書也找不到馮，他才會在媒體前嚴厲譴責基泰。李四川回憶說道，直至10日上午才聯繫到馮先勉，雙方約好9時30分到台北市政府開會，在會同法制局後達成後續的3點承諾。王淺秋詢問，發生事故當晚，工地主任介紹馮先勉後，馮有無過來稍微討論一下發生什麼事？還是馮就在旁邊像個路人一樣圍觀？李四川回應，馮先勉有過來打招呼說自己是總經理，但沒談任何相關事宜。李四川提及當天搶救的緊急過程，當時第一時間緊急疏散住戶且擴大預防性疏散，也聽到消防局回報工地一直傳出有「啪啪啪」聲音，察覺不妥後就要求立即消防局疏散住民，同時也詢問單號住戶對面有無房子間隔，獲得對面還有一排雙號住戶，因此當下就下令對面的也要依法全部撤離，並請區公所找到實踐大學先行安置。李四川當天到現場約22時，當時單號棟已有稍微傾斜、但未沉下去，便立即要求消防局、衛工處、水處全部灌水，看能不能讓基地平衡，不過隨「啪啪啪」間隔時間越來越短，他就要求全部站在旁邊的人全部快疏散。李表示，他在現場約40分鐘後，因灌水無法讓基地平衡，眼睜睜看著房子沉陷，垮掉就等同連續壁全部斷掉，緊急改為灌漿處理。李四川也提及退休後又重新回到北市府工作，很多市政幾乎都不陌生，不過比較麻煩的是極端氣候的影響，市區很多側溝的設計是無法承受近來的豪大雨，若「用工程的技術去追」不斷投入資源改善，怎樣都無法追上老天給的挑戰，舉例豪大雨對一些老舊、低窪的社區，市府要想辦法減災，這也是他回到北市府任職最大的考驗。</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>['陳世銘', '建商', '陳怡君', '檢察官', '台北', '基泰建設', '大直', '王世堅', '地層下陷', '殺人未遂']</t>
+          <t>['台北', '地層下陷', '馮先勉', '基泰建設', '李四川', '大直']</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -4080,125 +4080,15 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>屏縣農地不利耕地設綠能 環保局：發電量800MW非無限制擴張</t>
+          <t>陽光行動／光電來了 老農嘆「不但要吃土，連農保都沒有了」</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>生活</t>
+          <t>要聞</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
-        <is>
-          <t>〔記者陳彥廷／屏東報導〕屏東縣政府於東港、林邊、佳冬及枋寮4個沿海鄉鎮，劃定「嚴重地層下陷區光電計畫」專區，為確保農民耕作權，不過，近來坊間質疑聲浪漸漲，環保局強調，該區計畫發電量為800MW（百萬瓦），不會無限制擴張，因此至少會仍有3000公頃以上的農地可供農作。
-地面型光電場成為選戰攻防議題，屏東因沿海嚴重地層下陷區為全國首個縣府核淮得設光電案場專案，成在野黨攻詰對象，近期坊間又再傳出農民因種電失去農保、老農退場又留不住青農及蛇鼠窩藏副作用等爭議。
-屏縣府環保局指出，這4鄉鎮過去因超抽地下水，曾列為嚴重地層下陷區，現仍屬第1、2級地下水管制區，且在海水上溯下，許多土地都已出現鹽化，不少已是不利耕地多年，因此有縣府在尊重地主利用土地意願及權益前提及既有電力設施併網上限條件下，有限度的推動光電專區，預計發電量為800MW。
-環保局指出，在部分農地轉作太陽光電後，減少農民抽取林邊溪下游地下水需求，並搭配上游設置大潮州人工湖補注地下水，減緩地層下陷，達到國土復育及產業永續發展目的。而近年同樣大小的光電板發電效率已較八八風災後的「養水種電」到近2倍，單一片就可發電達400w，以目前併網約300MW太陽光電裝置容量，使用農地比例約250公頃左右，未來達到目標的在單位發電量更大下，所需面積的比例一定更小。至少會有3000公頃以上的農地可供農作使用。另外，對於無力管理田間工作，又有土地鹽化等不利因素無法耕作的年邁老農，則可以有穩定收入過退休生活。
-至於農保問題，環保局重申，農地若有意願出租供人種電，一定要進行變更地目，但這是完全基於地主的利用土地意願及權益，縣府環保局從未要求廠商提供所謂「不利耕作同意書」或其他網路媒體謠傳不平等條約相關文件，先前更製作地主注意事項手冊及Q&amp;A圖卡，公告於縣府綠辦官網，讓地主了解相關權利與義務，只要民眾對合約有疑問，均可撥打專線電話詢問綠能專案推動辦公室。針對部分地區爭議案件，在未取得居民同意之前，縣府已要求業者停止施工。
-蛇鼠患問題，縣府環保局長顏幸苑則認為，作物收成期間食物充沛易引鼠、鳥禽覓食，但太陽能案場內並無食源，應非屬引鼠主因，縣府要求專案輔導業者維護周遭環境整潔；至於選址不當，縣府重申，屏東縣綠能推動政策以「專案專區計畫」、「土地複合式利用」兩大策略為主，專案為有限度使用相對不適合耕種的土地發展綠能，專案專區外鄉鎮優先鼓勵結合既有設施與光電的「複合利用」方式。
-屏東縣環保局表示，民眾對於光電發展與環境保護議題逐漸重視，縣府尊重私有地主有處置自家土地財產，以及業者依法申請案件的權利，惟審查過程將審慎關注山坡地、耕作農地、歷史遺跡、生態保育或重要觀光景點聯絡道路沿線等議題，並要求廠商提出因應作為，以避免衍生爭議性問題，兼顧開發合理性及維護本縣農民耕作權益。</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr"/>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>2024/01/08</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>ltn</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>回響／屏東種電惹議 縣府強調非無限制開發仍有農地可耕</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>要聞</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>聯合報陽光行動專題報導光電進駐屏東，種電範圍遍及農地、山區到有文資價值的二戰遺跡，造成家園地景地貌變遷，衝擊老農生計、變相迫遷青農，更被地方形容為「惡鄰」，產生蛇鼠與害蟲，提升鄰田管理困難度，還潛藏糧食危機。 縣府環保局長顏幸苑表示，光電不會無限擴張，目前種電專區仍有約3千公頃可耕作並專案輔導業者除草，一定會兼顧農業永續發展。
-顏幸苑表示，台電饋線有上限規定，目前在既有的電力設施併網上限下，有限度的推動光電專區，不會無限制使用農地種電，而東港鎮、林邊、佳冬、枋寮鄉等4鄉鎮專案截至去年底，共併網約3百兆瓦光電，該區農地總面積約有3800公頃，至少還有約3千公頃面積可農作，使用農地比例不到4鄉鎮農地總面積一成。
-她強調，從未要求廠商提供「不利耕作同意書」或其他不平等條約相關文件，針對部分地區爭議案件，在未取得居民同意之前，皆已要求業者停止施工，另太陽能案場內並無食物來源，應非屬引來老鼠的主因，目前已要求專案輔導業者定期進行除草，維護周遭環境整潔。
-她指出，屏東綠能推動政策以「專案專區計畫」、「土地複合式利用」等2大策略為優先，有限度使用相對不適合耕種的土地發展綠能，提供給地主、農民階段性活化土地新選擇，對於無力管理田間工作，又有土地鹽化等不利因素無法耕作的年邁老農，則可以有穩定收入過退休生活。至於非專案專區的鄉鎮，則優先鼓勵廠商以「土地複合式利用」方式，利用既有設施結合太陽光電設施，有效利用公共空間。
-屏縣府綠能辦公室表示，尊重私有地主有處置自家土地財產，及業者依法申請案件的權利，相關審查過程將審慎關注山坡地、耕作農地、歷史遺跡、生態保育或重要觀光景點聯絡道路沿線等議題，並要求廠商提出因應作為，以避免衍生爭議性問題，兼顧開發合理性及維護本縣農民耕作權益。
-生利能源表示，屏東枋寮案場是合法開發，於2020年9月於案場內發現碉堡等歷史遺構後，隨即保留並主動展開一連串文資保護作為，並無二戰槍堡被挖除等情事。</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>['地層下陷', '屏東縣', '農地']</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>2024/01/08</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>udn</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>陽光行動／屏東瘋種電…家園變貌 老農離農、青農迫遷</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>要聞</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>從國道三號林邊交流道下來，光電場廣告映入眼簾；從大馬路旁到鄉間農田，光電板無所不在。這是屏東沿海地區這幾年興起的違和景致，也是全台種電縮影。在地青農批政府、業者聯手種電種到失心瘋，從農地、山區到有文資價值的二戰遺跡都不放過，不僅家園變貌，也迫使老農離農、變相迫遷青農。
-屏東農地種光電原是全台濫觴和典範，二○○九年八月莫拉克風災挾帶破紀錄雨量，造成中南部嚴重水災，也重創屏東南部沿海鄉鎮，不少魚塭、果園被沖毀。時任屏東縣長曹啟鴻提出「養水種電」計畫，縣府媒合魚塭、農地租給光電業者，地主負責管理，地主按月收地租及管理費，綠電賣給台電，能涵養地下水、減緩下陷，一舉數得。
-屏東種電 侵蝕農地 製表／都會地方中心
-農業部前身農委會二○一三年修法，允許不適耕作農地種電，大開種電之門，但農地非農用的罵聲不斷。二○一八年十月起，屏縣府公告實施「嚴重地層下陷地區土地活化暨太陽光電發電業整體規劃發展計畫」，開放下陷區農地可變更種電。
-二○二○年七月，農委會加嚴農地變更種電門檻，二到卅公頃農地變更要由中央審查，兩公頃以下原則不同意變更種電。但早在二○一八年屏東縣長潘孟安任內，報請行政院同意把東港、林邊、佳冬、枋寮四鄉鎮，畫為嚴重地層下陷區作光電專區，成為特例。
-四年多來，屏東種電發展快速，原本立意良善的光電，如今變成農民的陰霾。枋寮女青農張靜玉說，為衝高綠電占比，種電已種到失心瘋，不該種電的地方都被光電板占領，很多農民被業者遊說簽「不利耕作聲明書」，離農坐收光電場租金，但這些農地都種著蓮霧、水稻、芭樂，何來不利耕作？
-「沿海四鄉鎮美麗的鄉間景致丕變，綠地逐漸蒸發。」屏東縣環境保護聯盟理事長洪輝祥說，綠地、果園被一塊塊光電板取代，像貼狗皮膏藥般醜陋，不但壓縮農業空間，光電板遮陽廿年，農地將失去地力，衝擊農產業服務鏈，受益的是少數地主，受影響的是多數農民，整體農業將衰退，屆時想回頭搶救就難了。
-屏東縣府綠能辦公室表示，沿海四鄉鎮持續下陷，列第一、二級地下水管制區，縣府把四鄉鎮部分農地轉作光電場，搭配上游補注地下水，減緩地層下陷，創造地主、業者、政府、全民與綠能「五贏」，前年已達成綠電供應全縣民生用電的階段性目標。</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>['地層下陷', '潘孟安', '種電', '蓮霧', '農地', '農委會', '農業部', '農民', '青農']</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>2024/01/08</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>udn</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>陽光行動／光電來了 老農嘆「不但要吃土，連農保都沒有了」</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>要聞</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
         <is>
           <t>屏東是光電場熱區之一，正上演光電板與農民搶地爭奪戰。光電業者挨家挨戶以誘人租金勸說地主租地種電，租地種蓮霧的果農只能忍痛看著心血被毀，也斬斷兒子想當青農接班的願望。青農自嘲說，政府寧可把地租給業者種電，也不給老農一畝田維生，青年若當「漂鳥」回農村，肯定變走投無路的「落翅仔」。
 五十六歲鄭明偉在林邊、佳冬鄉租下三座蓮霧園，他說，有兩座花了十多年整理，收成正漸入佳境，地主竟收回種電，他只能忍痛放棄；由於種蓮霧要手把手長期培養技術，正在念農校的兒子雖有心接手，但他勸兒子算了，最好另謀出路。
@@ -4215,11 +4105,121 @@
 台大農經碩士張靜玉是枋寮蓮霧農，眼看鄰近農民被光電搶地，她忿忿不平，直指當年農委會主委蘇嘉全還推漂鳥計畫，要青年返鄉務農，現在連地都租不到，「這不是迫遷青農去都市討生活嗎？漂鳥回農村，恐怕走投無路變落翅仔吧！」</t>
         </is>
       </c>
-      <c r="D114" t="inlineStr">
+      <c r="D111" t="inlineStr">
         <is>
           <t>['國產署', '地層下陷', '種電', '蓮霧', '補償金', '農地', '農會', '農民', '電商']</t>
         </is>
       </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>2024/01/08</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>陽光行動／屏東瘋種電…家園變貌 老農離農、青農迫遷</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>要聞</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>從國道三號林邊交流道下來，光電場廣告映入眼簾；從大馬路旁到鄉間農田，光電板無所不在。這是屏東沿海地區這幾年興起的違和景致，也是全台種電縮影。在地青農批政府、業者聯手種電種到失心瘋，從農地、山區到有文資價值的二戰遺跡都不放過，不僅家園變貌，也迫使老農離農、變相迫遷青農。
+屏東農地種光電原是全台濫觴和典範，二○○九年八月莫拉克風災挾帶破紀錄雨量，造成中南部嚴重水災，也重創屏東南部沿海鄉鎮，不少魚塭、果園被沖毀。時任屏東縣長曹啟鴻提出「養水種電」計畫，縣府媒合魚塭、農地租給光電業者，地主負責管理，地主按月收地租及管理費，綠電賣給台電，能涵養地下水、減緩下陷，一舉數得。
+屏東種電 侵蝕農地 製表／都會地方中心
+農業部前身農委會二○一三年修法，允許不適耕作農地種電，大開種電之門，但農地非農用的罵聲不斷。二○一八年十月起，屏縣府公告實施「嚴重地層下陷地區土地活化暨太陽光電發電業整體規劃發展計畫」，開放下陷區農地可變更種電。
+二○二○年七月，農委會加嚴農地變更種電門檻，二到卅公頃農地變更要由中央審查，兩公頃以下原則不同意變更種電。但早在二○一八年屏東縣長潘孟安任內，報請行政院同意把東港、林邊、佳冬、枋寮四鄉鎮，畫為嚴重地層下陷區作光電專區，成為特例。
+四年多來，屏東種電發展快速，原本立意良善的光電，如今變成農民的陰霾。枋寮女青農張靜玉說，為衝高綠電占比，種電已種到失心瘋，不該種電的地方都被光電板占領，很多農民被業者遊說簽「不利耕作聲明書」，離農坐收光電場租金，但這些農地都種著蓮霧、水稻、芭樂，何來不利耕作？
+「沿海四鄉鎮美麗的鄉間景致丕變，綠地逐漸蒸發。」屏東縣環境保護聯盟理事長洪輝祥說，綠地、果園被一塊塊光電板取代，像貼狗皮膏藥般醜陋，不但壓縮農業空間，光電板遮陽廿年，農地將失去地力，衝擊農產業服務鏈，受益的是少數地主，受影響的是多數農民，整體農業將衰退，屆時想回頭搶救就難了。
+屏東縣府綠能辦公室表示，沿海四鄉鎮持續下陷，列第一、二級地下水管制區，縣府把四鄉鎮部分農地轉作光電場，搭配上游補注地下水，減緩地層下陷，創造地主、業者、政府、全民與綠能「五贏」，前年已達成綠電供應全縣民生用電的階段性目標。</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>['地層下陷', '潘孟安', '種電', '蓮霧', '農地', '農委會', '農業部', '農民', '青農']</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>2024/01/08</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>回響／屏東種電惹議 縣府強調非無限制開發仍有農地可耕</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>要聞</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>聯合報陽光行動專題報導光電進駐屏東，種電範圍遍及農地、山區到有文資價值的二戰遺跡，造成家園地景地貌變遷，衝擊老農生計、變相迫遷青農，更被地方形容為「惡鄰」，產生蛇鼠與害蟲，提升鄰田管理困難度，還潛藏糧食危機。 縣府環保局長顏幸苑表示，光電不會無限擴張，目前種電專區仍有約3千公頃可耕作並專案輔導業者除草，一定會兼顧農業永續發展。
+顏幸苑表示，台電饋線有上限規定，目前在既有的電力設施併網上限下，有限度的推動光電專區，不會無限制使用農地種電，而東港鎮、林邊、佳冬、枋寮鄉等4鄉鎮專案截至去年底，共併網約3百兆瓦光電，該區農地總面積約有3800公頃，至少還有約3千公頃面積可農作，使用農地比例不到4鄉鎮農地總面積一成。
+她強調，從未要求廠商提供「不利耕作同意書」或其他不平等條約相關文件，針對部分地區爭議案件，在未取得居民同意之前，皆已要求業者停止施工，另太陽能案場內並無食物來源，應非屬引來老鼠的主因，目前已要求專案輔導業者定期進行除草，維護周遭環境整潔。
+她指出，屏東綠能推動政策以「專案專區計畫」、「土地複合式利用」等2大策略為優先，有限度使用相對不適合耕種的土地發展綠能，提供給地主、農民階段性活化土地新選擇，對於無力管理田間工作，又有土地鹽化等不利因素無法耕作的年邁老農，則可以有穩定收入過退休生活。至於非專案專區的鄉鎮，則優先鼓勵廠商以「土地複合式利用」方式，利用既有設施結合太陽光電設施，有效利用公共空間。
+屏縣府綠能辦公室表示，尊重私有地主有處置自家土地財產，及業者依法申請案件的權利，相關審查過程將審慎關注山坡地、耕作農地、歷史遺跡、生態保育或重要觀光景點聯絡道路沿線等議題，並要求廠商提出因應作為，以避免衍生爭議性問題，兼顧開發合理性及維護本縣農民耕作權益。
+生利能源表示，屏東枋寮案場是合法開發，於2020年9月於案場內發現碉堡等歷史遺構後，隨即保留並主動展開一連串文資保護作為，並無二戰槍堡被挖除等情事。</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>['地層下陷', '屏東縣', '農地']</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>2024/01/08</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>udn</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>屏縣農地不利耕地設綠能 環保局：發電量800MW非無限制擴張</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>生活</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>〔記者陳彥廷／屏東報導〕屏東縣政府於東港、林邊、佳冬及枋寮4個沿海鄉鎮，劃定「嚴重地層下陷區光電計畫」專區，為確保農民耕作權，不過，近來坊間質疑聲浪漸漲，環保局強調，該區計畫發電量為800MW（百萬瓦），不會無限制擴張，因此至少會仍有3000公頃以上的農地可供農作。
+地面型光電場成為選戰攻防議題，屏東因沿海嚴重地層下陷區為全國首個縣府核淮得設光電案場專案，成在野黨攻詰對象，近期坊間又再傳出農民因種電失去農保、老農退場又留不住青農及蛇鼠窩藏副作用等爭議。
+屏縣府環保局指出，這4鄉鎮過去因超抽地下水，曾列為嚴重地層下陷區，現仍屬第1、2級地下水管制區，且在海水上溯下，許多土地都已出現鹽化，不少已是不利耕地多年，因此有縣府在尊重地主利用土地意願及權益前提及既有電力設施併網上限條件下，有限度的推動光電專區，預計發電量為800MW。
+環保局指出，在部分農地轉作太陽光電後，減少農民抽取林邊溪下游地下水需求，並搭配上游設置大潮州人工湖補注地下水，減緩地層下陷，達到國土復育及產業永續發展目的。而近年同樣大小的光電板發電效率已較八八風災後的「養水種電」到近2倍，單一片就可發電達400w，以目前併網約300MW太陽光電裝置容量，使用農地比例約250公頃左右，未來達到目標的在單位發電量更大下，所需面積的比例一定更小。至少會有3000公頃以上的農地可供農作使用。另外，對於無力管理田間工作，又有土地鹽化等不利因素無法耕作的年邁老農，則可以有穩定收入過退休生活。
+至於農保問題，環保局重申，農地若有意願出租供人種電，一定要進行變更地目，但這是完全基於地主的利用土地意願及權益，縣府環保局從未要求廠商提供所謂「不利耕作同意書」或其他網路媒體謠傳不平等條約相關文件，先前更製作地主注意事項手冊及Q&amp;A圖卡，公告於縣府綠辦官網，讓地主了解相關權利與義務，只要民眾對合約有疑問，均可撥打專線電話詢問綠能專案推動辦公室。針對部分地區爭議案件，在未取得居民同意之前，縣府已要求業者停止施工。
+蛇鼠患問題，縣府環保局長顏幸苑則認為，作物收成期間食物充沛易引鼠、鳥禽覓食，但太陽能案場內並無食源，應非屬引鼠主因，縣府要求專案輔導業者維護周遭環境整潔；至於選址不當，縣府重申，屏東縣綠能推動政策以「專案專區計畫」、「土地複合式利用」兩大策略為主，專案為有限度使用相對不適合耕種的土地發展綠能，專案專區外鄉鎮優先鼓勵結合既有設施與光電的「複合利用」方式。
+屏東縣環保局表示，民眾對於光電發展與環境保護議題逐漸重視，縣府尊重私有地主有處置自家土地財產，以及業者依法申請案件的權利，惟審查過程將審慎關注山坡地、耕作農地、歷史遺跡、生態保育或重要觀光景點聯絡道路沿線等議題，並要求廠商提出因應作為，以避免衍生爭議性問題，兼顧開發合理性及維護本縣農民耕作權益。</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr">
         <is>
           <t>2024/01/08</t>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>udn</t>
+          <t>ltn</t>
         </is>
       </c>
     </row>
@@ -4423,61 +4423,61 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
+          <t>北市慶城街路坍險吞4車！ 工地崩塌範圍完成回填</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr"/>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>台北市松山區慶城街一處新建工地旁，昨天晚間發生路面塌陷意外，經過將近20小時的搶救，工地內崩塌範圍已完成回填，今天下午也開始灌漿工地外圍的塌陷路面。初步研判，疑似是新建工程拆除建地既有的地下建築結構時，挖到不連續的弱面，才導致導溝崩塌。台北市松山區慶城街新建工地23日晚間發生地層坍陷意外，經過約18小時的緊急搶救，工地外圍崩塌範圍終於展開回填作業。從制高點俯瞰更清楚，混泥土車來回進出灌漿沒停過，因為這一崩，不僅人行道嚴重下陷，路邊車格也消失一大半，當時還有4輛汽車差點被吞噬。附近住戶直言，「好意外，真的很意外！文華飯店當初蓋的時候這麼近，也沒有發生過問題。」精華地段的豪宅新建案出現大坍塌，讓附近居民全都嚇壞，畢竟這長約4公尺、寬約30公尺，深度達到1.5公尺的坍陷範圍實在不小，而且建案甚至才正準備施作連續壁，基礎地基都還沒大規模開挖，竟然就在前置的導溝作業發生意外。初步研判，坍塌原因跟建地原先存在的地下室結構脫不了關係，原來這回要建立深導溝，越過既有結構時，卻不慎碰到既存的不連續面，才會釀禍。台北市土木技師公會理事長莊均緯指出，「破除既有的連續壁跟外牆，那個地方有個不連續面，原有的地下室這個部分，外牆它推擠進來變位，就把原來深導溝的側壁壓變形之後，就產生這樣的崩塌現象。」台北市長蔣萬安週六上午也二度到現場勘查，向居民保證，周邊住宅暫無安全疑慮，「在西側、南側、北側目前比對的監測數值是正常，而且也都沒有地面塌陷以及鄰房傾斜的狀況。」建管處則緊急開罰18萬，並勒令停工，後續就待道路回填，並由透地雷達確認周邊無安全疑慮，就可恢復通車，還給居民安全環境。</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>['工地崩塌', '慶城街', '地層下陷']</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>2024/02/24</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>ttv</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
           <t>北市工地地層下陷頻傳 柯文哲：高危險區應做必要措施</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr">
+      <c r="B122" t="inlineStr">
         <is>
           <t>地方</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr">
+      <c r="C122" t="inlineStr">
         <is>
           <t>台北市慶城街一處新建工地昨晚發生地層下陷事故，對於台北市接連發生地層下陷事件，前台北市長、民眾黨主席柯文哲今天表示，台北市本來就是地層下陷潛勢區，台北市政府已經把地圖做得很完整，要先知道高危險區，並做必要的措施。
 柯文哲表示，台北市本來就是地層下陷潛勢區，其實只要去工務局往上查一下，就可以看到地層下陷潛勢區有好幾個，因為這個地方本來就是盆地，所以就會有這個問題，目前台北市做的地圖已經相當完整，高危險區要事先知道，做出必要的措施。</t>
         </is>
       </c>
-      <c r="D121" t="inlineStr">
+      <c r="D122" t="inlineStr">
         <is>
           <t>['北市', '地層下陷', '柯文哲']</t>
         </is>
       </c>
-      <c r="E121" t="inlineStr">
+      <c r="E122" t="inlineStr">
         <is>
           <t>2024/02/24</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr">
+      <c r="F122" t="inlineStr">
         <is>
           <t>udn</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>北市慶城街路坍險吞4車！ 工地崩塌範圍完成回填</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr"/>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>台北市松山區慶城街一處新建工地旁，昨天晚間發生路面塌陷意外，經過將近20小時的搶救，工地內崩塌範圍已完成回填，今天下午也開始灌漿工地外圍的塌陷路面。初步研判，疑似是新建工程拆除建地既有的地下建築結構時，挖到不連續的弱面，才導致導溝崩塌。台北市松山區慶城街新建工地23日晚間發生地層坍陷意外，經過約18小時的緊急搶救，工地外圍崩塌範圍終於展開回填作業。從制高點俯瞰更清楚，混泥土車來回進出灌漿沒停過，因為這一崩，不僅人行道嚴重下陷，路邊車格也消失一大半，當時還有4輛汽車差點被吞噬。附近住戶直言，「好意外，真的很意外！文華飯店當初蓋的時候這麼近，也沒有發生過問題。」精華地段的豪宅新建案出現大坍塌，讓附近居民全都嚇壞，畢竟這長約4公尺、寬約30公尺，深度達到1.5公尺的坍陷範圍實在不小，而且建案甚至才正準備施作連續壁，基礎地基都還沒大規模開挖，竟然就在前置的導溝作業發生意外。初步研判，坍塌原因跟建地原先存在的地下室結構脫不了關係，原來這回要建立深導溝，越過既有結構時，卻不慎碰到既存的不連續面，才會釀禍。台北市土木技師公會理事長莊均緯指出，「破除既有的連續壁跟外牆，那個地方有個不連續面，原有的地下室這個部分，外牆它推擠進來變位，就把原來深導溝的側壁壓變形之後，就產生這樣的崩塌現象。」台北市長蔣萬安週六上午也二度到現場勘查，向居民保證，周邊住宅暫無安全疑慮，「在西側、南側、北側目前比對的監測數值是正常，而且也都沒有地面塌陷以及鄰房傾斜的狀況。」建管處則緊急開罰18萬，並勒令停工，後續就待道路回填，並由透地雷達確認周邊無安全疑慮，就可恢復通車，還給居民安全環境。</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>['工地崩塌', '慶城街', '地層下陷']</t>
-        </is>
-      </c>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>2024/02/24</t>
-        </is>
-      </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>ttv</t>
         </is>
       </c>
     </row>
@@ -4788,20 +4788,17 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>新北萬里加投溫泉地層下陷 封閉修繕</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>生活</t>
-        </is>
-      </c>
+          <t>疑地層下陷 萬里加投公共浴室封閉檢測</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr"/>
       <c r="C133" t="inlineStr">
         <is>
-          <t>〔記者俞肇福／新北報導〕日治時代建造的新北市萬里區加投溫泉公共浴室，因係屬免費泡湯，不但金山萬里當地民眾喜愛，就連基隆人也搭車專程前來免費泡湯；因日前發現疑似有地層下陷，萬里區公所立即封閉浴室，並邀請專業技師與工程廠商勘查，將於完成改善並確認無危險，才會再行開放。
-新北市議員周雅玲表示，她接獲當地民眾反映，加投溫泉公共浴室屋頂漏水、排水不良、牆有裂縫等事宜，廠商到場會勘後發現，懷疑是地層下陷，為確保民眾泡湯安全，自3月4日起先封閉浴室，經技師以透地雷達探測後，在男女湯室地底下有土壤流失現象，公所再度發起現勘，商討後續改善辦法。
-周雅玲指出，萬里加投溫泉公共浴室在10多年前曾經修繕，當時就曾經有出動透地雷達探測，這次透地雷達探測，與當年比較發現問題較為嚴重；她建議應該邀請土木技師一併會勘，包含溫泉主管機關的經濟發展局、水利局邀請來，對於周邊的溫泉開發應予以總量管制，以免加投溫泉公共浴室慘遭池魚之殃。
-萬里區區長黃雱勉表示，加投溫泉公共浴室經專業技師檢視，發現有下陷致建築物傾斜情形，為瞭解確切原因，找出有效的改善方法，公所將再請新北市土木技師公會等相關專家進行專業的檢查評估，期望在確保安全無虞的前提下，儘早恢復提供民眾泡湯空間。她呼籲，加投溫泉公共浴室封閉期間，民眾切勿擅闖翻越圍籬進入使用，以維護自身安全。</t>
+          <t>新北萬里的加頭溫泉2月份被遊客發現，不僅燈管、溫度顯示氣等等設備有問題，更有地層下陷，因此趕緊請公所找人檢修，目前已經緊急封閉，確認沒有安全疑慮，才會再度開放。
+浴池內整塊磁磚脫落，地磚也不平，甚至還有些地層下陷，看起來相當老舊，這裡是新北萬里的加頭溫泉，從日據時代起，就受到不少民眾喜愛，許多人泡完湯，都覺得放鬆筋骨。
+不過2月份卻被發現，不僅燈管，溫度顯示器，和一些溫泉管線設備有問題外，還有地層下陷的跡象，鐵鋁罐放在地上，都會不自主的，滾向一邊，加上後方就是溫泉露頭，要是坍方相當危險，萬里區長黃雱勉：「技師建議我們，要有專業的技師公會去，針對結構物下陷狀況，去做監測，評估後續是不是可以用，液壓灌漿的部分做改善。」
+地質人員透過地雷達偵測結果發現，確實男女湯內地底，有大量孔隙，造成土壤流失，目前公所已經，緊急封閉浴室，以民眾安全為第一考量，盡快修建。
+（封面圖／東森新聞）</t>
         </is>
       </c>
       <c r="D133" t="inlineStr"/>
@@ -4812,21 +4809,23 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>ltn</t>
+          <t>yahoo</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>萬里加投溫泉公共浴室疑地層下陷 封閉修繕中 (圖)</t>
+          <t>萬里加投溫泉公共浴室疑地層下陷 公所封閉修繕</t>
         </is>
       </c>
       <c r="B134" t="inlineStr"/>
       <c r="C134" t="inlineStr">
         <is>
-          <t>新北市萬里區加投溫泉公共浴室疑似有地層下陷的現象，為確保泡湯安全，目前已封閉修繕中。（公所提供）
-中央社記者王鴻國傳真 113年3月26日</t>
+          <t>萬里區公所以訊息說明，萬里區加投溫泉公共浴室於日據時代建造，歷史悠久，屬於海底溫泉，為當地居民從小到大泡湯空間。
+區公所表示，因2月底有民眾反應浴室內的燈管、溫度顯示器不亮等問題，於是委託廠商勘查後發現，疑似有地層下陷的現象，為確保泡湯安全，已封閉浴室。
+區長黃雱勉表示，為瞭解確切原因，找出有效的改善方法，將邀請專業技師進行檢查評估，以商討後續改善辦法，期望在安全的前提下，儘早恢復提供民眾泡湯空間。提醒民眾封閉期間勿擅自進入使用，以維護自身安全。
+萬里區公所主任秘書許明富向中央社記者表示，當地過去地層下陷、並完成改善多年，未影響溫泉的供給及溫度，加投溫泉公共浴室經找技師以透地雷達探測後，在男女湯室地下發現有土壤流失現象，未來將進行修繕改善，並確認無危險之虞，才會再行開放供民眾使用。（編輯：林恕暉）1130326</t>
         </is>
       </c>
       <c r="D134" t="inlineStr"/>
@@ -4844,13 +4843,14 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>地層下陷地面傾斜 萬里加投溫泉公共浴室暫封閉｜#鏡新聞</t>
+          <t>萬里加投溫泉公共浴室出現裂縫 疑地層下陷 (圖)</t>
         </is>
       </c>
       <c r="B135" t="inlineStr"/>
       <c r="C135" t="inlineStr">
         <is>
-          <t>新北市萬里的「加投溫泉」公共浴室，算是古蹟了。它是日據時期就蓋好的，而且到現在也有很多人，喜歡來這裡泡湯。不過上個月開始，這裡出現大大小小問題：浴池磁磚掉落、水泥柱有裂痕、地面也嚴重傾斜！因此現在浴池已經暫時封閉了，等到廠商都修繕完畢、確認安全都沒問題，才會再度開放。 （鏡新聞已上架86台，若無法收看，請洽詢當地系統台） 鏡新聞APP iOS👉https://reurl.cc/kqyqML 鏡新聞APP Android👉https://reurl.cc/Ay2y63 有話鏡來講YT👉https://reurl.cc/A4DjQj 少年新聞週記YT👉https://reurl.cc/K4DeN9</t>
+          <t>新北市萬里區公所表示，有民眾日前反應加投溫泉公共浴室內的燈管、溫度顯示器不亮等問題，委託廠商勘查後發現，疑似有地層下陷的現象。圖為建物出現裂縫。（公所提供）
+中央社記者王鴻國傳真 113年3月26日</t>
         </is>
       </c>
       <c r="D135" t="inlineStr"/>
@@ -4868,36 +4868,11 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>疑地層下陷 萬里加投溫泉公共浴室受損 (圖)</t>
+          <t>萬里加投溫泉地層下陷 地面傾斜急封閉</t>
         </is>
       </c>
       <c r="B136" t="inlineStr"/>
       <c r="C136" t="inlineStr">
-        <is>
-          <t>新北市萬里區加投溫泉公共浴室疑似有地層下陷的現象，造成浴池受損、壁磚脫落，未來將進行修繕改善，確認無危險之虞，才會再行開放供民眾使用。（公所提供）
-中央社記者王鴻國傳真 113年3月26日</t>
-        </is>
-      </c>
-      <c r="D136" t="inlineStr"/>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>2024/03/26</t>
-        </is>
-      </c>
-      <c r="F136" t="inlineStr">
-        <is>
-          <t>yahoo</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>萬里加投溫泉地層下陷 地面傾斜急封閉</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr"/>
-      <c r="C137" t="inlineStr">
         <is>
           <t>新北市萬里加投溫泉公共浴室歷史悠久，吸引許多人前來泡湯。不過，今年2月，有民眾反應溫泉設備出問題，沒想到廠商進場維修後，發現浴池磁磚掉落、水泥柱充滿裂痕、地面嚴重傾斜等狀況，更仔細勘查下，竟然有地層下陷的現象。地質檢測人員檢查，原來湯室的地底有大量孔隙，造成土壤流失，目前封閉整修。
 鋁罐放在地上一路滾不停，不只地面嚴重傾斜，浴池還有一大片磁磚脫落，水泥柱也充滿裂痕，原來這處溫泉發生地層下陷。
@@ -4909,6 +4884,37 @@
 公所強調儘快修建完成，提供民眾安全舒適的泡湯空間。</t>
         </is>
       </c>
+      <c r="D136" t="inlineStr"/>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>2024/03/26</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>新北萬里加投溫泉地層下陷 封閉修繕</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>生活</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>〔記者俞肇福／新北報導〕日治時代建造的新北市萬里區加投溫泉公共浴室，因係屬免費泡湯，不但金山萬里當地民眾喜愛，就連基隆人也搭車專程前來免費泡湯；因日前發現疑似有地層下陷，萬里區公所立即封閉浴室，並邀請專業技師與工程廠商勘查，將於完成改善並確認無危險，才會再行開放。
+新北市議員周雅玲表示，她接獲當地民眾反映，加投溫泉公共浴室屋頂漏水、排水不良、牆有裂縫等事宜，廠商到場會勘後發現，懷疑是地層下陷，為確保民眾泡湯安全，自3月4日起先封閉浴室，經技師以透地雷達探測後，在男女湯室地底下有土壤流失現象，公所再度發起現勘，商討後續改善辦法。
+周雅玲指出，萬里加投溫泉公共浴室在10多年前曾經修繕，當時就曾經有出動透地雷達探測，這次透地雷達探測，與當年比較發現問題較為嚴重；她建議應該邀請土木技師一併會勘，包含溫泉主管機關的經濟發展局、水利局邀請來，對於周邊的溫泉開發應予以總量管制，以免加投溫泉公共浴室慘遭池魚之殃。
+萬里區區長黃雱勉表示，加投溫泉公共浴室經專業技師檢視，發現有下陷致建築物傾斜情形，為瞭解確切原因，找出有效的改善方法，公所將再請新北市土木技師公會等相關專家進行專業的檢查評估，期望在確保安全無虞的前提下，儘早恢復提供民眾泡湯空間。她呼籲，加投溫泉公共浴室封閉期間，民眾切勿擅闖翻越圍籬進入使用，以維護自身安全。</t>
+        </is>
+      </c>
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="inlineStr">
         <is>
@@ -4917,24 +4923,20 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>yahoo</t>
+          <t>ltn</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>疑地層下陷 萬里加投公共浴室封閉檢測</t>
+          <t>地層下陷地面傾斜 萬里加投溫泉公共浴室暫封閉｜#鏡新聞</t>
         </is>
       </c>
       <c r="B138" t="inlineStr"/>
       <c r="C138" t="inlineStr">
         <is>
-          <t>新北萬里的加頭溫泉2月份被遊客發現，不僅燈管、溫度顯示氣等等設備有問題，更有地層下陷，因此趕緊請公所找人檢修，目前已經緊急封閉，確認沒有安全疑慮，才會再度開放。
-浴池內整塊磁磚脫落，地磚也不平，甚至還有些地層下陷，看起來相當老舊，這裡是新北萬里的加頭溫泉，從日據時代起，就受到不少民眾喜愛，許多人泡完湯，都覺得放鬆筋骨。
-不過2月份卻被發現，不僅燈管，溫度顯示器，和一些溫泉管線設備有問題外，還有地層下陷的跡象，鐵鋁罐放在地上，都會不自主的，滾向一邊，加上後方就是溫泉露頭，要是坍方相當危險，萬里區長黃雱勉：「技師建議我們，要有專業的技師公會去，針對結構物下陷狀況，去做監測，評估後續是不是可以用，液壓灌漿的部分做改善。」
-地質人員透過地雷達偵測結果發現，確實男女湯內地底，有大量孔隙，造成土壤流失，目前公所已經，緊急封閉浴室，以民眾安全為第一考量，盡快修建。
-（封面圖／東森新聞）</t>
+          <t>新北市萬里的「加投溫泉」公共浴室，算是古蹟了。它是日據時期就蓋好的，而且到現在也有很多人，喜歡來這裡泡湯。不過上個月開始，這裡出現大大小小問題：浴池磁磚掉落、水泥柱有裂痕、地面也嚴重傾斜！因此現在浴池已經暫時封閉了，等到廠商都修繕完畢、確認安全都沒問題，才會再度開放。 （鏡新聞已上架86台，若無法收看，請洽詢當地系統台） 鏡新聞APP iOS👉https://reurl.cc/kqyqML 鏡新聞APP Android👉https://reurl.cc/Ay2y63 有話鏡來講YT👉https://reurl.cc/A4DjQj 少年新聞週記YT👉https://reurl.cc/K4DeN9</t>
         </is>
       </c>
       <c r="D138" t="inlineStr"/>
@@ -4952,16 +4954,14 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>萬里加投溫泉公共浴室疑地層下陷 公所封閉修繕</t>
+          <t>萬里加投溫泉公共浴室疑地層下陷 封閉修繕中 (圖)</t>
         </is>
       </c>
       <c r="B139" t="inlineStr"/>
       <c r="C139" t="inlineStr">
         <is>
-          <t>萬里區公所以訊息說明，萬里區加投溫泉公共浴室於日據時代建造，歷史悠久，屬於海底溫泉，為當地居民從小到大泡湯空間。
-區公所表示，因2月底有民眾反應浴室內的燈管、溫度顯示器不亮等問題，於是委託廠商勘查後發現，疑似有地層下陷的現象，為確保泡湯安全，已封閉浴室。
-區長黃雱勉表示，為瞭解確切原因，找出有效的改善方法，將邀請專業技師進行檢查評估，以商討後續改善辦法，期望在安全的前提下，儘早恢復提供民眾泡湯空間。提醒民眾封閉期間勿擅自進入使用，以維護自身安全。
-萬里區公所主任秘書許明富向中央社記者表示，當地過去地層下陷、並完成改善多年，未影響溫泉的供給及溫度，加投溫泉公共浴室經找技師以透地雷達探測後，在男女湯室地下發現有土壤流失現象，未來將進行修繕改善，並確認無危險之虞，才會再行開放供民眾使用。（編輯：林恕暉）1130326</t>
+          <t>新北市萬里區加投溫泉公共浴室疑似有地層下陷的現象，為確保泡湯安全，目前已封閉修繕中。（公所提供）
+中央社記者王鴻國傳真 113年3月26日</t>
         </is>
       </c>
       <c r="D139" t="inlineStr"/>
@@ -4979,13 +4979,13 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>萬里加投溫泉公共浴室出現裂縫 疑地層下陷 (圖)</t>
+          <t>疑地層下陷 萬里加投溫泉公共浴室受損 (圖)</t>
         </is>
       </c>
       <c r="B140" t="inlineStr"/>
       <c r="C140" t="inlineStr">
         <is>
-          <t>新北市萬里區公所表示，有民眾日前反應加投溫泉公共浴室內的燈管、溫度顯示器不亮等問題，委託廠商勘查後發現，疑似有地層下陷的現象。圖為建物出現裂縫。（公所提供）
+          <t>新北市萬里區加投溫泉公共浴室疑似有地層下陷的現象，造成浴池受損、壁磚脫落，未來將進行修繕改善，確認無危險之虞，才會再行開放供民眾使用。（公所提供）
 中央社記者王鴻國傳真 113年3月26日</t>
         </is>
       </c>
@@ -5423,11 +5423,81 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
+          <t>中國正在下沉中 !  45％城市每年下陷超過3公釐</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>財經</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>中國過度抽取地下水，導致近40%主要城市的土地下陷。（路透）
+陳麗珠／核稿編輯
+〔財經頻道／綜合報導〕中國有近一半的主要城市正遭受「中度至重度」不等程度的沉降，在海平面上升的情況下，恐有數百萬人將面臨洪水風險。《路透》指出，中國都市人口約9億人，當中約有2.7億人生活在每年下陷逾3公釐的地區，相當於都市人口的29%。
+在中國82個城市中，約有45%每年下沉超過3公釐、16%土地平均每年下沉更是超過10公釐，約有6700萬居民生活於此。研究小組指出，由於中國城市人口多，即使是一小部分地層下陷，也可能造成重大威脅。
+據了解，而造成中國土地逐年下沉，最主要是地下水位下降所致。
+路透表示，「土地下陷」對中國每年造成超過75億元人民幣（約新台幣337億元）的損失。研究人員預計，在下個世紀內，中國將有約近四分之一的沿海土地，恐低於海平面，數億人將面臨大洪水風險。
+最嚴重的受災城市是北方的天津，這城市約有1500萬人口。2023年一場「突發地質災害」，導致3000名居民被疏散，調查人員將這場災害歸咎於，水資源枯竭和地熱井的建設。
+一手掌握經濟脈動點我訂閱自由財經Youtube頻道</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr"/>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>2024/04/19</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>ltn</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>中國下沉中！研究指4成主要城市土地正下陷 上有2.7億人居住</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>最新一份根據衛星雷達觀測的研究顯示，中國近40%主要城市的土地正發生「中度至重度」的地層下陷，上億居民面臨洪水的風險；加上海平面上升，上海、廣州、天津都面臨災害風險。
+綜合路透社與美國有線電視新聞網（CNN）報導，這篇研究今天（4/19）發表在期刊《科學》（Science）上。由中國華南師範大學教授敖祖銳領軍的研究小組，透過衛星雷達觀測中國82個主要城市在2015至2022年的地層下陷情況，發現40%城市土地每年平均下沉超過3公釐。
+中國都市人口約9億，約有2.7億人口生活在這些每年下陷逾3公釐的地區，相當於都市人口的29%。
+這82個城市中，更有16%土地平均每年下沉超過10公釐，6700萬居民生活於此。研究小組指出，由於中國城市人口多，即使是一小部分地層下陷，也可能造成重大威脅。
+導致中國都市地層下陷的主因是過度抽用地下水，另一大因素是城市土地上的重量不斷增加。在時間推移下，沉積物堆積、以及不斷增加的沉重建物，將土壤越壓越緊實，導致土地下沉。
+研究顯示，由於地層下陷和海平面上升，最終中國將有約四分之一的沿岸地帶將低於海平面，天津、上海、廣州周邊都面臨這樣的風險。
+中國一些地區已經建立保護措施，這份研究並未探討這些措施的效果。報告合著者、北京大學城市與環境學院教授陶勝利說，上海就建造了數公尺高的堤防，「即使地層下陷和海平面上升，這樣龐大的沿海堤防也能在很大程度上降低城市被淹沒的風險」，就他所知，沒有其他國家打造過規模這麼大的堤防。
+陶勝利稱，中國政府也實施嚴格的地下水管制法規，減緩了上海周邊的地層下陷速度。
+全球多個城市都在下陷
+維吉尼亞理工大學博士後研究員奧恩亨（Leonard Ohenhen）最近一份針對美國地層下陷狀況的報告指出，大部分城市都會發生土地下沉，但因為沿海地區有海平面上升的問題，大家比較關心沿海城市，「但大多數城市下沉的速度，和沿海城市其實都差不多、甚至還更快」。
+地層下陷也不僅是中國才有的問題。CNN指出，美國紐約市等數十個沿海城市正在下沉；墨西哥首都墨西哥城，土地每年最多下沉50公分，可能是全球沉最快的；荷蘭已有25%土地低於海平面。
+今年2月另一項研究指出，全球約630萬平方公里的土地有下陷風險，印尼是最嚴重的國家之一，首都雅加達大部分地區現在都已低於海平面。新加坡2022年一項研究提到，全球面臨嚴重地層下陷的44個沿海大城市當中，有30個在亞洲。</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>2024/04/19</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
           <t>遭9億人口重壓！研究：中國近半主要城市正在下陷</t>
         </is>
       </c>
-      <c r="B154" t="inlineStr"/>
-      <c r="C154" t="inlineStr">
+      <c r="B156" t="inlineStr"/>
+      <c r="C156" t="inlineStr">
         <is>
           <t>路透社報導，根據今天(19日)發布的一份全國衛星資料研究顯示，中國將近一半的主要城市正遭受「中等到嚴重」程度的地層下陷，數百萬人將面臨洪災風險，尤其海平面正在上升。
 這篇發表於《科學》(Science)期刊的論文作者發現，中國45%的都市土地正以每年超過3公釐的速度下陷，16%的都市土地下陷速度每年超過10公釐，造成的原因不僅是地下水位下降，還有建築環境的龐大重量。
@@ -5443,76 +5513,6 @@
 羅德島大學(University of Rhode Island)地球物理學專家魏馬特(Matt Wei)表示：「這是一個都市化和人口增長的問題，人口密度愈大，抽的水就愈多，也就造成更多下陷。」</t>
         </is>
       </c>
-      <c r="D154" t="inlineStr"/>
-      <c r="E154" t="inlineStr">
-        <is>
-          <t>2024/04/19</t>
-        </is>
-      </c>
-      <c r="F154" t="inlineStr">
-        <is>
-          <t>yahoo</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>中國正在下沉中 !  45％城市每年下陷超過3公釐</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>財經</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>中國過度抽取地下水，導致近40%主要城市的土地下陷。（路透）
-陳麗珠／核稿編輯
-〔財經頻道／綜合報導〕中國有近一半的主要城市正遭受「中度至重度」不等程度的沉降，在海平面上升的情況下，恐有數百萬人將面臨洪水風險。《路透》指出，中國都市人口約9億人，當中約有2.7億人生活在每年下陷逾3公釐的地區，相當於都市人口的29%。
-在中國82個城市中，約有45%每年下沉超過3公釐、16%土地平均每年下沉更是超過10公釐，約有6700萬居民生活於此。研究小組指出，由於中國城市人口多，即使是一小部分地層下陷，也可能造成重大威脅。
-據了解，而造成中國土地逐年下沉，最主要是地下水位下降所致。
-路透表示，「土地下陷」對中國每年造成超過75億元人民幣（約新台幣337億元）的損失。研究人員預計，在下個世紀內，中國將有約近四分之一的沿海土地，恐低於海平面，數億人將面臨大洪水風險。
-最嚴重的受災城市是北方的天津，這城市約有1500萬人口。2023年一場「突發地質災害」，導致3000名居民被疏散，調查人員將這場災害歸咎於，水資源枯竭和地熱井的建設。
-一手掌握經濟脈動點我訂閱自由財經Youtube頻道</t>
-        </is>
-      </c>
-      <c r="D155" t="inlineStr"/>
-      <c r="E155" t="inlineStr">
-        <is>
-          <t>2024/04/19</t>
-        </is>
-      </c>
-      <c r="F155" t="inlineStr">
-        <is>
-          <t>ltn</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>中國下沉中！研究指4成主要城市土地正下陷 上有2.7億人居住</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr"/>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>最新一份根據衛星雷達觀測的研究顯示，中國近40%主要城市的土地正發生「中度至重度」的地層下陷，上億居民面臨洪水的風險；加上海平面上升，上海、廣州、天津都面臨災害風險。
-綜合路透社與美國有線電視新聞網（CNN）報導，這篇研究今天（4/19）發表在期刊《科學》（Science）上。由中國華南師範大學教授敖祖銳領軍的研究小組，透過衛星雷達觀測中國82個主要城市在2015至2022年的地層下陷情況，發現40%城市土地每年平均下沉超過3公釐。
-中國都市人口約9億，約有2.7億人口生活在這些每年下陷逾3公釐的地區，相當於都市人口的29%。
-這82個城市中，更有16%土地平均每年下沉超過10公釐，6700萬居民生活於此。研究小組指出，由於中國城市人口多，即使是一小部分地層下陷，也可能造成重大威脅。
-導致中國都市地層下陷的主因是過度抽用地下水，另一大因素是城市土地上的重量不斷增加。在時間推移下，沉積物堆積、以及不斷增加的沉重建物，將土壤越壓越緊實，導致土地下沉。
-研究顯示，由於地層下陷和海平面上升，最終中國將有約四分之一的沿岸地帶將低於海平面，天津、上海、廣州周邊都面臨這樣的風險。
-中國一些地區已經建立保護措施，這份研究並未探討這些措施的效果。報告合著者、北京大學城市與環境學院教授陶勝利說，上海就建造了數公尺高的堤防，「即使地層下陷和海平面上升，這樣龐大的沿海堤防也能在很大程度上降低城市被淹沒的風險」，就他所知，沒有其他國家打造過規模這麼大的堤防。
-陶勝利稱，中國政府也實施嚴格的地下水管制法規，減緩了上海周邊的地層下陷速度。
-全球多個城市都在下陷
-維吉尼亞理工大學博士後研究員奧恩亨（Leonard Ohenhen）最近一份針對美國地層下陷狀況的報告指出，大部分城市都會發生土地下沉，但因為沿海地區有海平面上升的問題，大家比較關心沿海城市，「但大多數城市下沉的速度，和沿海城市其實都差不多、甚至還更快」。
-地層下陷也不僅是中國才有的問題。CNN指出，美國紐約市等數十個沿海城市正在下沉；墨西哥首都墨西哥城，土地每年最多下沉50公分，可能是全球沉最快的；荷蘭已有25%土地低於海平面。
-今年2月另一項研究指出，全球約630萬平方公里的土地有下陷風險，印尼是最嚴重的國家之一，首都雅加達大部分地區現在都已低於海平面。新加坡2022年一項研究提到，全球面臨嚴重地層下陷的44個沿海大城市當中，有30個在亞洲。</t>
-        </is>
-      </c>
       <c r="D156" t="inlineStr"/>
       <c r="E156" t="inlineStr">
         <is>
@@ -5681,66 +5681,11 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>高鐵路段監測雲林段累積下陷114.2公分 鐵道局：結構安全</t>
+          <t>高鐵雲林段累積下陷114.2公分 鐵道局：結構安全</t>
         </is>
       </c>
       <c r="B162" t="inlineStr"/>
       <c r="C162" t="inlineStr">
-        <is>
-          <t>台灣高鐵公司從民國92年至今，委託學術單位，持續每年定期針對高鐵沿線結構墩柱下陷進行監測，並提報交通部，鐵道局日前公布2023年監測報告。根據最新報告，高鐵彰化、雲林路段下陷持續，高鐵路線最大累積下陷量已達到114.2公分，位於雲林縣土庫鎮台78線與高鐵交界處的墩柱，但自103年進行改善工程後，目標範圍內的墩柱差異沉陷量呈逐年降低的趨勢。
-監測報告顯示，2023年的高鐵彰化、雲林共8處路段的下陷量從2.6公分（彰化溪洲）到5.4公分（雲林縣土庫鎮與元長鄉交界），都比2022年增加，嘉義不但未再下陷，還連續2年回脹，但2023年的回脹量比2022年少。
-鐵道局說，較值得關注的高鐵下陷路段，包括：彰化溪州高鐵與中山高跨交、高鐵雲林車站區、高鐵跨雲158縣道、高鐵跨台78號快速道路，與高鐵行車安全有關的橋墩間差異沉陷所累積角變量，目前皆在容許範圍內（連續梁為1/1500、簡支梁1/1000），高鐵結構安全無虞。
-鐵道局說，高鐵有零星數處的累積角變量有逾容許範圍的橋墩（結構型式皆為簡支梁），台灣高鐵已納入定期軌道巡檢及土建設施維護計畫，持續密切關注，並依角變量變化速率，按風險等級高低，採取相應加密監測頻率，並已備妥軌道調整及預防性結構補強方案。根據監測報告，目前高鐵累積角變量過標準值的橋墩，反而是位在沉陷改善的嘉義路段，位在朴子溪河中，目前簡支梁累積的角變量達1.96/1000，而朴子溪北岸簡支梁累積角變量為0.395/1000，雖仍在容許值範圍，但已從2020年起逐年增加。</t>
-        </is>
-      </c>
-      <c r="D162" t="inlineStr"/>
-      <c r="E162" t="inlineStr">
-        <is>
-          <t>2024/04/29</t>
-        </is>
-      </c>
-      <c r="F162" t="inlineStr">
-        <is>
-          <t>yahoo</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>基泰大直未按圖施工坍塌　建築師等5人遭起訴</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr"/>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>基泰建設位在台北市大直的新建案在去（2023）年9月7日晚間突然發生崩塌，導致附近5樓民宅下陷成4樓，台北地檢署偵查終結，將工地邱姓負責人、基泰公司工程部人員張姓工地主任、王姓及劉姓建築師、姜姓專案人員等5人，依涉犯違背建築術成規、偽造文書等罪起訴。檢方查出，大直基泰建案坍塌後，所幸住戶及時撤離，無人傷亡，檢方發現建案商未依圖施工，應該60公分厚的連續壁，只施作50公分。此外，建商為了趕工，改變施工順序，竟調整監測異常數據，導致工安意外，至於基泰董事長陳世銘等2人被控殺人未遂部分則予以簽結。</t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>['地層下陷', '基泰建設', '工安意外', '建案', '偽造文書']</t>
-        </is>
-      </c>
-      <c r="E163" t="inlineStr">
-        <is>
-          <t>2024/04/29</t>
-        </is>
-      </c>
-      <c r="F163" t="inlineStr">
-        <is>
-          <t>mirrormedia</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>高鐵雲林段累積下陷114.2公分 鐵道局：結構安全</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr"/>
-      <c r="C164" t="inlineStr">
         <is>
           <t>（中央社記者汪淑芬台北29日電）根據鐵道局新公布的台灣高鐵路段下陷監測報告，彰化、雲林下陷持續，累積下陷量最大的是雲林114.2公分。鐵道局表示，高鐵墩柱角變量都在容許範圍內，結構安全無虞。
 高鐵路線通過彰化、雲林及嘉義主要地層下陷區，台灣高鐵公司從民國92年至今，委託學術單位，持續每年定期針對高鐵沿線結構墩柱下陷進行監測，並提報交通部，鐵道局日前公布112年監測報告。
@@ -5751,7 +5696,62 @@
 根據監測報告，目前高鐵累積角變量超過標準值的橋墩，反而是在沉陷改善的嘉義路段，位於朴子溪河中，目前簡支梁累積角變量達1.96/1000；而朴子溪北岸簡支梁累積角變量為0.395/1000，雖仍在容許值範圍，但已從109年起逐年增加。（編輯：張雅淨）1130429</t>
         </is>
       </c>
-      <c r="D164" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>2024/04/29</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>高鐵路段監測雲林段累積下陷114.2公分 鐵道局：結構安全</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr"/>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>台灣高鐵公司從民國92年至今，委託學術單位，持續每年定期針對高鐵沿線結構墩柱下陷進行監測，並提報交通部，鐵道局日前公布2023年監測報告。根據最新報告，高鐵彰化、雲林路段下陷持續，高鐵路線最大累積下陷量已達到114.2公分，位於雲林縣土庫鎮台78線與高鐵交界處的墩柱，但自103年進行改善工程後，目標範圍內的墩柱差異沉陷量呈逐年降低的趨勢。
+監測報告顯示，2023年的高鐵彰化、雲林共8處路段的下陷量從2.6公分（彰化溪洲）到5.4公分（雲林縣土庫鎮與元長鄉交界），都比2022年增加，嘉義不但未再下陷，還連續2年回脹，但2023年的回脹量比2022年少。
+鐵道局說，較值得關注的高鐵下陷路段，包括：彰化溪州高鐵與中山高跨交、高鐵雲林車站區、高鐵跨雲158縣道、高鐵跨台78號快速道路，與高鐵行車安全有關的橋墩間差異沉陷所累積角變量，目前皆在容許範圍內（連續梁為1/1500、簡支梁1/1000），高鐵結構安全無虞。
+鐵道局說，高鐵有零星數處的累積角變量有逾容許範圍的橋墩（結構型式皆為簡支梁），台灣高鐵已納入定期軌道巡檢及土建設施維護計畫，持續密切關注，並依角變量變化速率，按風險等級高低，採取相應加密監測頻率，並已備妥軌道調整及預防性結構補強方案。根據監測報告，目前高鐵累積角變量過標準值的橋墩，反而是位在沉陷改善的嘉義路段，位在朴子溪河中，目前簡支梁累積的角變量達1.96/1000，而朴子溪北岸簡支梁累積角變量為0.395/1000，雖仍在容許值範圍，但已從2020年起逐年增加。</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr"/>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>2024/04/29</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>基泰大直未按圖施工坍塌　建築師等5人遭起訴</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr"/>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>基泰建設位在台北市大直的新建案在去（2023）年9月7日晚間突然發生崩塌，導致附近5樓民宅下陷成4樓，台北地檢署偵查終結，將工地邱姓負責人、基泰公司工程部人員張姓工地主任、王姓及劉姓建築師、姜姓專案人員等5人，依涉犯違背建築術成規、偽造文書等罪起訴。檢方查出，大直基泰建案坍塌後，所幸住戶及時撤離，無人傷亡，檢方發現建案商未依圖施工，應該60公分厚的連續壁，只施作50公分。此外，建商為了趕工，改變施工順序，竟調整監測異常數據，導致工安意外，至於基泰董事長陳世銘等2人被控殺人未遂部分則予以簽結。</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>['地層下陷', '基泰建設', '工安意外', '建案', '偽造文書']</t>
+        </is>
+      </c>
       <c r="E164" t="inlineStr">
         <is>
           <t>2024/04/29</t>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>yahoo</t>
+          <t>mirrormedia</t>
         </is>
       </c>
     </row>
@@ -6017,34 +6017,6 @@
       <c r="B173" t="inlineStr"/>
       <c r="C173" t="inlineStr">
         <is>
-          <t>根據環境部、國科會發布全球暖化若未來無法有效控制增溫，台灣夏天可能長達7個月，海平面上升會造成海岸溢淹面積增加，其中以雲林溢淹面積增加最顯著，對此雲縣府水利處表示，除了暖化影響，地層下陷也是影響主因，目前四湖箔子寮漁港配合中央提出因應計畫。雲林縣最大箔子寮漁港，去（2023）年8月發生嚴重海水倒灌，整座漁港幾乎都被淹沒，甚至危及近鄰村落。根據環境部、國科會報告指出，若全球暖化未來無法有效控制增溫，未來海平面上升會再造成海岸溢淹，又以雲林最嚴重。雲林縣水利處長許宏博提及，「以大數據來看幾十年，可能就只有上升1到2公分，相對地層下陷的因素，這可能是較小影響程度，不過因應整個地層下陷或是海洋暖化海平面上升，這是雲林縣必須去克服。」雲縣府水利處表示，除暖化影響海岸溢淹面積，雲林縣面對最大危機是地層下陷，1年在內陸地區有平均5至6公分下陷、沿海地區平均2至3公分下陷，現在針對四湖箔子寮漁港也提出因應。許宏博說明，「較低地方我就會蓋一個類似牆，然後去墊高，讓它們潮位來時不會溢到內陸裡面，都擋在防潮牆之外。」水利處表示，若海平面上升淹水面積自然加大，經盤點雲林四湖箔子寮漁港比較危急，去年9月經中央、地方共同會勘後，將花3500萬元加高碼頭港岸，以防海水再入侵，整個工程預計再半年可完工。</t>
-        </is>
-      </c>
-      <c r="D173" t="inlineStr">
-        <is>
-          <t>['地層下陷', '水利處', '全球暖化', '雲林縣', '漁港']</t>
-        </is>
-      </c>
-      <c r="E173" t="inlineStr">
-        <is>
-          <t>2024/05/10</t>
-        </is>
-      </c>
-      <c r="F173" t="inlineStr">
-        <is>
-          <t>pts</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>全球暖化將致雲林溢淹顯著 水利處：地層下陷也是主因</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr"/>
-      <c r="C174" t="inlineStr">
-        <is>
           <t>根據環境部、國科會報告指出，若全球暖化未來無法有效控制增溫，未來海平面上升會再造成海岸溢淹，又以雲林最嚴重。
 雲林縣水利處長許宏博提及，「以大數據來看幾十年，可能就只有上升1到2公分，相對地層下陷的因素，這可能是較小影響程度，不過因應整個地層下陷或是海洋暖化海平面上升，這是雲林縣必須去克服。」
 雲縣府水利處表示，除暖化影響海岸溢淹面積，雲林縣面對最大危機是地層下陷，1年在內陸地區有平均5至6公分下陷、沿海地區平均2至3公分下陷，現在針對四湖箔子寮漁港也提出因應。
@@ -6052,7 +6024,35 @@
 水利處表示，若海平面上升淹水面積自然加大，經盤點雲林四湖箔子寮漁港比較危急，去年9月經中央、地方共同會勘後，將花3500萬元加高碼頭港岸，以防海水再入侵，整個工程預計再半年可完工。</t>
         </is>
       </c>
-      <c r="D174" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>2024/05/10</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>全球暖化將致雲林溢淹顯著 水利處：地層下陷也是主因</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr"/>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>根據環境部、國科會發布全球暖化若未來無法有效控制增溫，台灣夏天可能長達7個月，海平面上升會造成海岸溢淹面積增加，其中以雲林溢淹面積增加最顯著，對此雲縣府水利處表示，除了暖化影響，地層下陷也是影響主因，目前四湖箔子寮漁港配合中央提出因應計畫。雲林縣最大箔子寮漁港，去（2023）年8月發生嚴重海水倒灌，整座漁港幾乎都被淹沒，甚至危及近鄰村落。根據環境部、國科會報告指出，若全球暖化未來無法有效控制增溫，未來海平面上升會再造成海岸溢淹，又以雲林最嚴重。雲林縣水利處長許宏博提及，「以大數據來看幾十年，可能就只有上升1到2公分，相對地層下陷的因素，這可能是較小影響程度，不過因應整個地層下陷或是海洋暖化海平面上升，這是雲林縣必須去克服。」雲縣府水利處表示，除暖化影響海岸溢淹面積，雲林縣面對最大危機是地層下陷，1年在內陸地區有平均5至6公分下陷、沿海地區平均2至3公分下陷，現在針對四湖箔子寮漁港也提出因應。許宏博說明，「較低地方我就會蓋一個類似牆，然後去墊高，讓它們潮位來時不會溢到內陸裡面，都擋在防潮牆之外。」水利處表示，若海平面上升淹水面積自然加大，經盤點雲林四湖箔子寮漁港比較危急，去年9月經中央、地方共同會勘後，將花3500萬元加高碼頭港岸，以防海水再入侵，整個工程預計再半年可完工。</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>['地層下陷', '水利處', '全球暖化', '雲林縣', '漁港']</t>
+        </is>
+      </c>
       <c r="E174" t="inlineStr">
         <is>
           <t>2024/05/10</t>
@@ -6060,7 +6060,7 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>yahoo</t>
+          <t>pts</t>
         </is>
       </c>
     </row>
@@ -6092,6 +6092,62 @@
         </is>
       </c>
     </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>空品全球最糟！ 雅加達人口密集+地層下陷 將遷首都｜#鏡新聞</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr"/>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>印尼打算遷移首都！因為目前的首都雅加達，問題一籮筐。除了人口過度密集，引發的「城市汙染」之外，當地還是：全球「地層下陷最快」的都市。當局計畫，兩年內就要在新首都：努山塔拉，蓋好機場，各項新建設，也讓不少台廠嗅到商機！來看到鏡新聞記者從印尼帶來的第一手觀察！ （鏡新聞已上架86台，若無法收看，請洽詢當地系統台） 鏡新聞APP iOS👉https://reurl.cc/kqyqML 鏡新聞APP Android👉https://reurl.cc/Ay2y63 有話鏡來講YT👉https://reurl.cc/A4DjQj 少年新聞週記YT👉https://reurl.cc/K4DeN9</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr"/>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>2024/05/19</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>印尼將啟動星鏈網路服務 馬斯克親赴峇里島啟用</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr"/>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>科技大亨馬斯克（Elon Musk）今天（5/19）抵達印尼峇里島，將與印尼總統佐科威（Joko Widodo）一起參加星鏈（Starlink）網路服務的啟用。印尼將是東南亞第三個使用星鏈服務的國家，政府希望星鏈能夠提高各島嶼的網路普及度；這是印尼一個月內迎接的第3名科技企業執行長，此前蘋果、微軟執行長都已來訪。
+綜合路透社與美聯社報導，太空科技公司SpaceX執行長馬斯克今天搭乘私人飛機抵達印尼峇里島機場，印尼首席投資部長盧胡特（Luhut Binsar Pandjaitan）在機場迎接。預計兩人將會討論一些重要的合作，包含星鏈服務的啟動，馬斯克還會簽署一項協助印尼加強衛生與教育單位聯絡互通的合約。
+盧胡特表示，馬斯克今天稍晚將和印尼總統佐科威一起在峇里島首府登巴薩（Denpasar）的社區衛生中心一起啟動星鏈。盧胡特說，在衛生機構啟動這項服務，呼應星鏈「提供平價高速網路」的宗旨，尤其是在網路收訊不佳或過於偏遠的地區。
+印尼是個群島國家，有約1.7萬座島嶼，橫跨3個時區，人口超過2.7億。盧胡特說，印尼偏鄉需要星鏈來拓展高速網路，尤其是要用來解決衛生、教育和海事單位的問題。
+印尼通訊部長布迪（Budi Arie Setiadi）上週表示，星鏈已經獲得在印尼營運許可。布迪強調，星鏈的低軌衛星可以讓網路擴及目前印尼通訊商無法到達的地區。
+據報，位於印尼婆羅洲（Borneo）的新首都努山塔拉（Nusantara）本月將先試用星鏈，8月正式上線；印尼正準備遷都努山塔拉，因為受海平面上升與地層下陷影響，預計目前的首都雅加達大部分地區將在2050年被淹沒。
+印尼將是東南亞第三個使用星鏈服務的國家。馬來西亞去年已核發許可證給營運星鏈的SpaceX公司，菲律賓一家公司則是在2022年與SpaceX簽約合作。
+在馬斯克訪印尼前，蘋果公司執行長庫克（Tim Cook）4月17也與印尼總統佐科威會面，並表示會將印尼的產能納入考慮；兩周後，微軟執行長納德拉（Satya Nadella）同月30日訪印尼，承諾未來4年內在印尼投資17億美元，強化印尼的新雲端運算與人工智慧基礎設施。
+馬斯克此次訪峇里島，也將參加第十屆世界水論壇（World Water Forum），研討全球水資源和衛生挑戰。</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr"/>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>2024/05/19</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>